<commit_message>
Auto commit - 2024-06-18
</commit_message>
<xml_diff>
--- a/2024/2024_06_07_CB_loans/2_Money_Base_dayly_eng.xlsx
+++ b/2024/2024_06_07_CB_loans/2_Money_Base_dayly_eng.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBDD3E8A-8335-4ECF-92AB-A311D93B3535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="605"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name=" Eng actual exchange rate" sheetId="4" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="143">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -528,11 +529,17 @@
   <si>
     <t>13.06.24</t>
   </si>
+  <si>
+    <t>14.06.24</t>
+  </si>
+  <si>
+    <t>17.06.24</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
@@ -1363,128 +1370,128 @@
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="122">
-    <cellStyle name=" Verticals" xfId="1"/>
-    <cellStyle name="_1_²ÜºÈÆø" xfId="2"/>
+    <cellStyle name=" Verticals" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="_1_²ÜºÈÆø" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="20% - Accent1" xfId="3" builtinId="30"/>
-    <cellStyle name="20% - Accent1 2" xfId="4"/>
-    <cellStyle name="20% - Accent2 2" xfId="5"/>
-    <cellStyle name="20% - Accent3 2" xfId="6"/>
-    <cellStyle name="20% - Accent4 2" xfId="7"/>
-    <cellStyle name="20% - Accent5 2" xfId="8"/>
-    <cellStyle name="20% - Accent6 2" xfId="9"/>
-    <cellStyle name="40% - Accent1 2" xfId="10"/>
-    <cellStyle name="40% - Accent2 2" xfId="11"/>
-    <cellStyle name="40% - Accent3 2" xfId="12"/>
-    <cellStyle name="40% - Accent4 2" xfId="13"/>
-    <cellStyle name="40% - Accent5 2" xfId="14"/>
-    <cellStyle name="40% - Accent6 2" xfId="15"/>
+    <cellStyle name="20% - Accent1 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="20% - Accent2 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="20% - Accent3 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="20% - Accent4 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="20% - Accent5 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="20% - Accent6 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="40% - Accent1 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="40% - Accent2 2" xfId="11" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="40% - Accent3 2" xfId="12" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="40% - Accent4 2" xfId="13" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="40% - Accent5 2" xfId="14" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="40% - Accent6 2" xfId="15" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
     <cellStyle name="60% - Accent1" xfId="16" builtinId="32"/>
-    <cellStyle name="60% - Accent1 2" xfId="17"/>
-    <cellStyle name="60% - Accent2 2" xfId="18"/>
-    <cellStyle name="60% - Accent3 2" xfId="19"/>
-    <cellStyle name="60% - Accent4 2" xfId="20"/>
-    <cellStyle name="60% - Accent5 2" xfId="21"/>
-    <cellStyle name="60% - Accent6 2" xfId="22"/>
-    <cellStyle name="Accent1 - 20%" xfId="23"/>
-    <cellStyle name="Accent1 - 40%" xfId="24"/>
-    <cellStyle name="Accent1 - 60%" xfId="25"/>
-    <cellStyle name="Accent1 2" xfId="26"/>
-    <cellStyle name="Accent2 - 20%" xfId="27"/>
-    <cellStyle name="Accent2 - 40%" xfId="28"/>
-    <cellStyle name="Accent2 - 60%" xfId="29"/>
-    <cellStyle name="Accent2 2" xfId="30"/>
-    <cellStyle name="Accent3 - 20%" xfId="31"/>
-    <cellStyle name="Accent3 - 40%" xfId="32"/>
-    <cellStyle name="Accent3 - 60%" xfId="33"/>
-    <cellStyle name="Accent3 2" xfId="34"/>
-    <cellStyle name="Accent4 - 20%" xfId="35"/>
-    <cellStyle name="Accent4 - 40%" xfId="36"/>
-    <cellStyle name="Accent4 - 60%" xfId="37"/>
-    <cellStyle name="Accent4 2" xfId="38"/>
-    <cellStyle name="Accent5 - 20%" xfId="39"/>
-    <cellStyle name="Accent5 - 40%" xfId="40"/>
-    <cellStyle name="Accent5 - 60%" xfId="41"/>
-    <cellStyle name="Accent5 2" xfId="42"/>
-    <cellStyle name="Accent6 - 20%" xfId="43"/>
-    <cellStyle name="Accent6 - 40%" xfId="44"/>
-    <cellStyle name="Accent6 - 60%" xfId="45"/>
-    <cellStyle name="Accent6 2" xfId="46"/>
-    <cellStyle name="al_laroux_7_laroux_1_²ðò²Ê´²ÜÎ" xfId="47"/>
-    <cellStyle name="Bad 2" xfId="48"/>
-    <cellStyle name="Body" xfId="49"/>
-    <cellStyle name="Calculation 2" xfId="50"/>
-    <cellStyle name="Check Cell 2" xfId="51"/>
+    <cellStyle name="60% - Accent1 2" xfId="17" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="60% - Accent2 2" xfId="18" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="60% - Accent3 2" xfId="19" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="60% - Accent4 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="60% - Accent5 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="60% - Accent6 2" xfId="22" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Accent1 - 20%" xfId="23" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="Accent1 - 40%" xfId="24" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Accent1 - 60%" xfId="25" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Accent1 2" xfId="26" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Accent2 - 20%" xfId="27" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="Accent2 - 40%" xfId="28" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Accent2 - 60%" xfId="29" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Accent2 2" xfId="30" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="Accent3 - 20%" xfId="31" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="Accent3 - 40%" xfId="32" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="Accent3 - 60%" xfId="33" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Accent3 2" xfId="34" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Accent4 - 20%" xfId="35" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="Accent4 - 40%" xfId="36" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="Accent4 - 60%" xfId="37" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="Accent4 2" xfId="38" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="Accent5 - 20%" xfId="39" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Accent5 - 40%" xfId="40" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="Accent5 - 60%" xfId="41" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Accent5 2" xfId="42" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Accent6 - 20%" xfId="43" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Accent6 - 40%" xfId="44" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Accent6 - 60%" xfId="45" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="Accent6 2" xfId="46" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="al_laroux_7_laroux_1_²ðò²Ê´²ÜÎ" xfId="47" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="Bad 2" xfId="48" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Body" xfId="49" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="Calculation 2" xfId="50" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="Check Cell 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
     <cellStyle name="Comma" xfId="52" builtinId="3"/>
-    <cellStyle name="Comma 2" xfId="53"/>
-    <cellStyle name="Comma 3" xfId="54"/>
-    <cellStyle name="Dezimal [0]_laroux" xfId="55"/>
-    <cellStyle name="Dezimal_laroux" xfId="56"/>
-    <cellStyle name="Emphasis 1" xfId="57"/>
-    <cellStyle name="Emphasis 2" xfId="58"/>
-    <cellStyle name="Emphasis 3" xfId="59"/>
-    <cellStyle name="Euro" xfId="60"/>
-    <cellStyle name="Explanatory Text 2" xfId="61"/>
-    <cellStyle name="Good 2" xfId="62"/>
-    <cellStyle name="Heading 1 2" xfId="63"/>
-    <cellStyle name="Heading 2 2" xfId="64"/>
-    <cellStyle name="Heading 3 2" xfId="65"/>
-    <cellStyle name="Heading 4 2" xfId="66"/>
-    <cellStyle name="Îáû÷íûé_AMD" xfId="67"/>
-    <cellStyle name="Input 2" xfId="68"/>
-    <cellStyle name="Linked Cell 2" xfId="69"/>
-    <cellStyle name="Milliers [0]_laroux" xfId="70"/>
-    <cellStyle name="Milliers_laroux" xfId="71"/>
-    <cellStyle name="Neutral 2" xfId="72"/>
-    <cellStyle name="no dec" xfId="73"/>
+    <cellStyle name="Comma 2" xfId="53" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="Comma 3" xfId="54" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="Dezimal [0]_laroux" xfId="55" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
+    <cellStyle name="Dezimal_laroux" xfId="56" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
+    <cellStyle name="Emphasis 1" xfId="57" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="Emphasis 2" xfId="58" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="Emphasis 3" xfId="59" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
+    <cellStyle name="Euro" xfId="60" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
+    <cellStyle name="Explanatory Text 2" xfId="61" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
+    <cellStyle name="Good 2" xfId="62" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
+    <cellStyle name="Heading 1 2" xfId="63" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
+    <cellStyle name="Heading 2 2" xfId="64" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
+    <cellStyle name="Heading 3 2" xfId="65" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
+    <cellStyle name="Heading 4 2" xfId="66" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
+    <cellStyle name="Îáû÷íûé_AMD" xfId="67" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
+    <cellStyle name="Input 2" xfId="68" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
+    <cellStyle name="Linked Cell 2" xfId="69" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
+    <cellStyle name="Milliers [0]_laroux" xfId="70" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
+    <cellStyle name="Milliers_laroux" xfId="71" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
+    <cellStyle name="Neutral 2" xfId="72" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
+    <cellStyle name="no dec" xfId="73" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal - Style1" xfId="74"/>
-    <cellStyle name="Normal 10" xfId="75"/>
-    <cellStyle name="Normal 10 2" xfId="76"/>
-    <cellStyle name="Normal 11" xfId="77"/>
-    <cellStyle name="Normal 11 2" xfId="78"/>
-    <cellStyle name="Normal 12" xfId="79"/>
-    <cellStyle name="Normal 12 2" xfId="80"/>
-    <cellStyle name="Normal 13" xfId="81"/>
-    <cellStyle name="Normal 13 2" xfId="82"/>
-    <cellStyle name="Normal 14" xfId="83"/>
-    <cellStyle name="Normal 14 2" xfId="84"/>
-    <cellStyle name="Normal 16" xfId="85"/>
-    <cellStyle name="Normal 17" xfId="86"/>
-    <cellStyle name="Normal 18" xfId="87"/>
-    <cellStyle name="Normal 19" xfId="88"/>
-    <cellStyle name="Normal 2 10" xfId="89"/>
-    <cellStyle name="Normal 2 11" xfId="90"/>
-    <cellStyle name="Normal 2 2" xfId="91"/>
-    <cellStyle name="Normal 2 3" xfId="92"/>
-    <cellStyle name="Normal 2 4" xfId="93"/>
-    <cellStyle name="Normal 2 5" xfId="94"/>
-    <cellStyle name="Normal 2 6" xfId="95"/>
-    <cellStyle name="Normal 2 7" xfId="96"/>
-    <cellStyle name="Normal 2 8" xfId="97"/>
-    <cellStyle name="Normal 2 9" xfId="98"/>
-    <cellStyle name="Normal 20" xfId="99"/>
-    <cellStyle name="Normal 21" xfId="100"/>
-    <cellStyle name="Normal 22" xfId="101"/>
-    <cellStyle name="Normal 23" xfId="102"/>
-    <cellStyle name="Normal 3 2" xfId="103"/>
-    <cellStyle name="Normal 5 2" xfId="104"/>
-    <cellStyle name="Normal 6 2" xfId="105"/>
-    <cellStyle name="Normal 7 2" xfId="106"/>
-    <cellStyle name="Normal_01_Jan_ 2010" xfId="107"/>
-    <cellStyle name="Note 2" xfId="108"/>
-    <cellStyle name="Output 2" xfId="109"/>
-    <cellStyle name="Percent 2" xfId="110"/>
-    <cellStyle name="Percent 3" xfId="111"/>
-    <cellStyle name="Sheet Title" xfId="112"/>
-    <cellStyle name="Standard_laroux" xfId="113"/>
-    <cellStyle name="Style 1" xfId="114"/>
-    <cellStyle name="Style 2" xfId="115"/>
-    <cellStyle name="Title 2" xfId="116"/>
-    <cellStyle name="Total 2" xfId="117"/>
-    <cellStyle name="ux" xfId="118"/>
-    <cellStyle name="Währung [0]_laroux" xfId="119"/>
-    <cellStyle name="Währung_laroux" xfId="120"/>
-    <cellStyle name="Warning Text 2" xfId="121"/>
+    <cellStyle name="Normal - Style1" xfId="74" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
+    <cellStyle name="Normal 10" xfId="75" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
+    <cellStyle name="Normal 10 2" xfId="76" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
+    <cellStyle name="Normal 11" xfId="77" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
+    <cellStyle name="Normal 11 2" xfId="78" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
+    <cellStyle name="Normal 12" xfId="79" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
+    <cellStyle name="Normal 12 2" xfId="80" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
+    <cellStyle name="Normal 13" xfId="81" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
+    <cellStyle name="Normal 13 2" xfId="82" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
+    <cellStyle name="Normal 14" xfId="83" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
+    <cellStyle name="Normal 14 2" xfId="84" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
+    <cellStyle name="Normal 16" xfId="85" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
+    <cellStyle name="Normal 17" xfId="86" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
+    <cellStyle name="Normal 18" xfId="87" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
+    <cellStyle name="Normal 19" xfId="88" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
+    <cellStyle name="Normal 2 10" xfId="89" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
+    <cellStyle name="Normal 2 11" xfId="90" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
+    <cellStyle name="Normal 2 2" xfId="91" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
+    <cellStyle name="Normal 2 3" xfId="92" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
+    <cellStyle name="Normal 2 4" xfId="93" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
+    <cellStyle name="Normal 2 5" xfId="94" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
+    <cellStyle name="Normal 2 6" xfId="95" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
+    <cellStyle name="Normal 2 7" xfId="96" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
+    <cellStyle name="Normal 2 8" xfId="97" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
+    <cellStyle name="Normal 2 9" xfId="98" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
+    <cellStyle name="Normal 20" xfId="99" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
+    <cellStyle name="Normal 21" xfId="100" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
+    <cellStyle name="Normal 22" xfId="101" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
+    <cellStyle name="Normal 23" xfId="102" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
+    <cellStyle name="Normal 3 2" xfId="103" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
+    <cellStyle name="Normal 5 2" xfId="104" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
+    <cellStyle name="Normal 6 2" xfId="105" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
+    <cellStyle name="Normal 7 2" xfId="106" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
+    <cellStyle name="Normal_01_Jan_ 2010" xfId="107" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
+    <cellStyle name="Note 2" xfId="108" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
+    <cellStyle name="Output 2" xfId="109" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
+    <cellStyle name="Percent 2" xfId="110" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
+    <cellStyle name="Percent 3" xfId="111" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
+    <cellStyle name="Sheet Title" xfId="112" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
+    <cellStyle name="Standard_laroux" xfId="113" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
+    <cellStyle name="Style 1" xfId="114" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
+    <cellStyle name="Style 2" xfId="115" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
+    <cellStyle name="Title 2" xfId="116" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
+    <cellStyle name="Total 2" xfId="117" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
+    <cellStyle name="ux" xfId="118" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
+    <cellStyle name="Währung [0]_laroux" xfId="119" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
+    <cellStyle name="Währung_laroux" xfId="120" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
+    <cellStyle name="Warning Text 2" xfId="121" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1643,6 +1650,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1678,6 +1702,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1853,14 +1894,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DJ59"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:DL59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="BL7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="DB7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="DL21" sqref="DL21"/>
+      <selection pane="bottomRight" activeCell="DT26" sqref="DT26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1876,27 +1917,27 @@
     <col min="65" max="84" width="16" style="7" hidden="1" customWidth="1"/>
     <col min="85" max="85" width="16" style="7" bestFit="1" customWidth="1"/>
     <col min="86" max="104" width="16" style="7" hidden="1" customWidth="1"/>
-    <col min="105" max="114" width="16" style="7" bestFit="1" customWidth="1"/>
-    <col min="115" max="16384" width="11.5703125" style="7"/>
+    <col min="105" max="116" width="16" style="7" bestFit="1" customWidth="1"/>
+    <col min="117" max="16384" width="11.5703125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:114" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:116" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:114" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:116" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:114" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:116" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
     </row>
-    <row r="4" spans="1:114" ht="3" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:116" ht="3" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
     </row>
-    <row r="5" spans="1:114" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:116" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -2239,8 +2280,14 @@
       <c r="DJ5" s="10" t="s">
         <v>140</v>
       </c>
+      <c r="DK5" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="DL5" s="10" t="s">
+        <v>142</v>
+      </c>
     </row>
-    <row r="6" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
@@ -2355,8 +2402,10 @@
       <c r="DH6" s="12"/>
       <c r="DI6" s="12"/>
       <c r="DJ6" s="12"/>
+      <c r="DK6" s="12"/>
+      <c r="DL6" s="12"/>
     </row>
-    <row r="7" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
@@ -2699,8 +2748,14 @@
       <c r="DJ7" s="13">
         <v>944324.80879325024</v>
       </c>
+      <c r="DK7" s="13">
+        <v>942500.65823890967</v>
+      </c>
+      <c r="DL7" s="13">
+        <v>939895.1588591066</v>
+      </c>
     </row>
-    <row r="8" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
@@ -3043,8 +3098,14 @@
       <c r="DJ8" s="13">
         <v>736860.47574674967</v>
       </c>
+      <c r="DK8" s="13">
+        <v>745918.73152969009</v>
+      </c>
+      <c r="DL8" s="13">
+        <v>743611.59776629356</v>
+      </c>
     </row>
-    <row r="9" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -3387,8 +3448,14 @@
       <c r="DJ9" s="13">
         <v>-397720.20520780003</v>
       </c>
+      <c r="DK9" s="13">
+        <v>-392458.82517259999</v>
+      </c>
+      <c r="DL9" s="13">
+        <v>-390767.90789720003</v>
+      </c>
     </row>
-    <row r="10" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
@@ -3731,8 +3798,14 @@
       <c r="DJ10" s="13">
         <v>669676.01526859985</v>
       </c>
+      <c r="DK10" s="13">
+        <v>670295.5266173</v>
+      </c>
+      <c r="DL10" s="13">
+        <v>669332.19195340003</v>
+      </c>
     </row>
-    <row r="11" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -4075,8 +4148,14 @@
       <c r="DJ11" s="13">
         <v>368082.05338499998</v>
       </c>
+      <c r="DK11" s="13">
+        <v>368164.106768</v>
+      </c>
+      <c r="DL11" s="13">
+        <v>368410.26691900002</v>
+      </c>
     </row>
-    <row r="12" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
@@ -4419,8 +4498,14 @@
       <c r="DJ12" s="13">
         <v>368082.05338499998</v>
       </c>
+      <c r="DK12" s="13">
+        <v>368164.106768</v>
+      </c>
+      <c r="DL12" s="13">
+        <v>368410.26691900002</v>
+      </c>
     </row>
-    <row r="13" spans="1:114" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:116" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -4763,8 +4848,14 @@
       <c r="DJ13" s="13">
         <v>0</v>
       </c>
+      <c r="DK13" s="13">
+        <v>0</v>
+      </c>
+      <c r="DL13" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
@@ -5107,8 +5198,14 @@
       <c r="DJ14" s="13">
         <v>0</v>
       </c>
+      <c r="DK14" s="13">
+        <v>0</v>
+      </c>
+      <c r="DL14" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
@@ -5451,8 +5548,14 @@
       <c r="DJ15" s="13">
         <v>0</v>
       </c>
+      <c r="DK15" s="13">
+        <v>0</v>
+      </c>
+      <c r="DL15" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
@@ -5795,8 +5898,14 @@
       <c r="DJ16" s="13">
         <v>0</v>
       </c>
+      <c r="DK16" s="13">
+        <v>0</v>
+      </c>
+      <c r="DL16" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
@@ -6139,8 +6248,14 @@
       <c r="DJ17" s="13">
         <v>0</v>
       </c>
+      <c r="DK17" s="13">
+        <v>0</v>
+      </c>
+      <c r="DL17" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
@@ -6483,8 +6598,14 @@
       <c r="DJ18" s="13">
         <v>0</v>
       </c>
+      <c r="DK18" s="13">
+        <v>0</v>
+      </c>
+      <c r="DL18" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
@@ -6827,8 +6948,14 @@
       <c r="DJ19" s="13">
         <v>0</v>
       </c>
+      <c r="DK19" s="13">
+        <v>0</v>
+      </c>
+      <c r="DL19" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:114" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:116" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>11</v>
       </c>
@@ -7171,8 +7298,14 @@
       <c r="DJ20" s="13">
         <v>0</v>
       </c>
+      <c r="DK20" s="13">
+        <v>0</v>
+      </c>
+      <c r="DL20" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
@@ -7515,8 +7648,14 @@
       <c r="DJ21" s="13">
         <v>0</v>
       </c>
+      <c r="DK21" s="13">
+        <v>0</v>
+      </c>
+      <c r="DL21" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -7859,8 +7998,14 @@
       <c r="DJ22" s="13">
         <v>464904.66568594985</v>
       </c>
+      <c r="DK22" s="13">
+        <v>468082.0300849902</v>
+      </c>
+      <c r="DL22" s="13">
+        <v>465047.31371009361</v>
+      </c>
     </row>
-    <row r="23" spans="1:114" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:116" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
         <v>4</v>
       </c>
@@ -8203,8 +8348,14 @@
       <c r="DJ23" s="21">
         <v>1681185.2845399999</v>
       </c>
+      <c r="DK23" s="21">
+        <v>1688419.3897685998</v>
+      </c>
+      <c r="DL23" s="21">
+        <v>1683506.7566254002</v>
+      </c>
     </row>
-    <row r="24" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>5</v>
       </c>
@@ -8547,8 +8698,14 @@
       <c r="DJ24" s="13">
         <v>887459.64008979988</v>
       </c>
+      <c r="DK24" s="13">
+        <v>889639.67366279999</v>
+      </c>
+      <c r="DL24" s="13">
+        <v>890811.5800357</v>
+      </c>
     </row>
-    <row r="25" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>14</v>
       </c>
@@ -8891,8 +9048,14 @@
       <c r="DJ25" s="13">
         <v>332363.24833640002</v>
       </c>
+      <c r="DK25" s="13">
+        <v>328355.24917009997</v>
+      </c>
+      <c r="DL25" s="13">
+        <v>327319.11003029998</v>
+      </c>
     </row>
-    <row r="26" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
@@ -9235,8 +9398,14 @@
       <c r="DJ26" s="13">
         <v>443093.39145390003</v>
       </c>
+      <c r="DK26" s="13">
+        <v>448837.34673009999</v>
+      </c>
+      <c r="DL26" s="13">
+        <v>447558.86425559997</v>
+      </c>
     </row>
-    <row r="27" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>6</v>
       </c>
@@ -9579,8 +9748,14 @@
       <c r="DJ27" s="13">
         <v>18269.004659899976</v>
       </c>
+      <c r="DK27" s="13">
+        <v>21587.120205599815</v>
+      </c>
+      <c r="DL27" s="13">
+        <v>17817.202303800208</v>
+      </c>
     </row>
-    <row r="28" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>7</v>
       </c>
@@ -9923,8 +10098,14 @@
       <c r="DJ28" s="13">
         <v>15610.266807100001</v>
       </c>
+      <c r="DK28" s="13">
+        <v>19564.9055974</v>
+      </c>
+      <c r="DL28" s="13">
+        <v>15441.157375000001</v>
+      </c>
     </row>
-    <row r="29" spans="1:114" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:116" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -10267,8 +10448,14 @@
       <c r="DJ29" s="13">
         <v>2658.7378527999999</v>
       </c>
+      <c r="DK29" s="13">
+        <v>2022.2146082000002</v>
+      </c>
+      <c r="DL29" s="13">
+        <v>2376.0449288000004</v>
+      </c>
     </row>
-    <row r="30" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
@@ -10383,8 +10570,10 @@
       <c r="DH30" s="14"/>
       <c r="DI30" s="14"/>
       <c r="DJ30" s="14"/>
+      <c r="DK30" s="14"/>
+      <c r="DL30" s="14"/>
     </row>
-    <row r="31" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>15</v>
       </c>
@@ -10501,8 +10690,10 @@
       <c r="DH31" s="15"/>
       <c r="DI31" s="15"/>
       <c r="DJ31" s="15"/>
+      <c r="DK31" s="15"/>
+      <c r="DL31" s="15"/>
     </row>
-    <row r="32" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
@@ -10617,8 +10808,10 @@
       <c r="DH32" s="16"/>
       <c r="DI32" s="16"/>
       <c r="DJ32" s="16"/>
+      <c r="DK32" s="16"/>
+      <c r="DL32" s="16"/>
     </row>
-    <row r="33" spans="1:114" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:116" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>19</v>
       </c>
@@ -10944,7 +11137,7 @@
         <v>-7222.5502792990301</v>
       </c>
       <c r="CE33" s="14">
-        <f t="shared" ref="CE33:DJ37" si="5">CE7-CD7</f>
+        <f t="shared" ref="CE33:DL37" si="5">CE7-CD7</f>
         <v>-2284.7872705847258</v>
       </c>
       <c r="CF33" s="14">
@@ -11071,8 +11264,16 @@
         <f t="shared" si="5"/>
         <v>8483.6479218938621</v>
       </c>
+      <c r="DK33" s="14">
+        <f t="shared" si="5"/>
+        <v>-1824.1505543405656</v>
+      </c>
+      <c r="DL33" s="14">
+        <f t="shared" si="5"/>
+        <v>-2605.4993798030773</v>
+      </c>
     </row>
-    <row r="34" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>22</v>
       </c>
@@ -11525,8 +11726,16 @@
         <f t="shared" si="5"/>
         <v>-2764.7294835938374</v>
       </c>
+      <c r="DK34" s="14">
+        <f t="shared" si="5"/>
+        <v>9058.255782940425</v>
+      </c>
+      <c r="DL34" s="14">
+        <f t="shared" si="5"/>
+        <v>-2307.1337633965304</v>
+      </c>
     </row>
-    <row r="35" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>2</v>
       </c>
@@ -11979,8 +12188,16 @@
         <f t="shared" si="5"/>
         <v>-1680.0291277000797</v>
       </c>
+      <c r="DK35" s="14">
+        <f t="shared" si="5"/>
+        <v>5261.3800352000399</v>
+      </c>
+      <c r="DL35" s="14">
+        <f t="shared" si="5"/>
+        <v>1690.9172753999592</v>
+      </c>
     </row>
-    <row r="36" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>3</v>
       </c>
@@ -12433,8 +12650,16 @@
         <f t="shared" si="5"/>
         <v>130.09935639984906</v>
       </c>
+      <c r="DK36" s="14">
+        <f t="shared" si="5"/>
+        <v>619.51134870015085</v>
+      </c>
+      <c r="DL36" s="14">
+        <f t="shared" si="5"/>
+        <v>-963.33466389996465</v>
+      </c>
     </row>
-    <row r="37" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>17</v>
       </c>
@@ -12887,8 +13112,16 @@
         <f t="shared" si="5"/>
         <v>82.053384999977425</v>
       </c>
+      <c r="DK37" s="14">
+        <f t="shared" si="5"/>
+        <v>82.053383000020403</v>
+      </c>
+      <c r="DL37" s="14">
+        <f t="shared" si="5"/>
+        <v>246.16015100001823</v>
+      </c>
     </row>
-    <row r="38" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>23</v>
       </c>
@@ -13210,7 +13443,7 @@
         <v>92.435473999998067</v>
       </c>
       <c r="CD38" s="14">
-        <f t="shared" ref="CD38:DJ42" si="9">CD12-CC12</f>
+        <f t="shared" ref="CD38:DL42" si="9">CD12-CC12</f>
         <v>84445.387153999996</v>
       </c>
       <c r="CE38" s="14">
@@ -13341,8 +13574,16 @@
         <f t="shared" si="9"/>
         <v>82.053384999977425</v>
       </c>
+      <c r="DK38" s="14">
+        <f t="shared" si="9"/>
+        <v>82.053383000020403</v>
+      </c>
+      <c r="DL38" s="14">
+        <f t="shared" si="9"/>
+        <v>246.16015100001823</v>
+      </c>
     </row>
-    <row r="39" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>24</v>
       </c>
@@ -13795,8 +14036,16 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="DK39" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DL39" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="40" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>25</v>
       </c>
@@ -14249,8 +14498,16 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="DK40" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DL40" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="41" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>26</v>
       </c>
@@ -14703,8 +14960,16 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="DK41" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DL41" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="42" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>9</v>
       </c>
@@ -15157,8 +15422,16 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="DK42" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DL42" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="43" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>10</v>
       </c>
@@ -15592,7 +15865,7 @@
         <v>0</v>
       </c>
       <c r="DF43" s="14">
-        <f t="shared" ref="DF43:DJ47" si="12">-(DF17-DE17)</f>
+        <f t="shared" ref="DF43:DL47" si="12">-(DF17-DE17)</f>
         <v>17003.135245900001</v>
       </c>
       <c r="DG43" s="14">
@@ -15611,8 +15884,16 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
+      <c r="DK43" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DL43" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="44" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>12</v>
       </c>
@@ -16065,8 +16346,16 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
+      <c r="DK44" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DL44" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="45" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>18</v>
       </c>
@@ -16519,8 +16808,16 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
+      <c r="DK45" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DL45" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="46" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>11</v>
       </c>
@@ -16973,8 +17270,16 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
+      <c r="DK46" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DL46" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="47" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>16</v>
       </c>
@@ -17427,8 +17732,16 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
+      <c r="DK47" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DL47" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>21</v>
       </c>
@@ -17722,7 +18035,7 @@
         <v>-3678.5371843058383</v>
       </c>
       <c r="BW48" s="14">
-        <f t="shared" ref="BW48:DJ50" si="18">BW22-BV22</f>
+        <f t="shared" ref="BW48:DL50" si="18">BW22-BV22</f>
         <v>-4079.5047014922602</v>
       </c>
       <c r="BX48" s="14">
@@ -17881,8 +18194,16 @@
         <f t="shared" si="18"/>
         <v>-1214.7997122935485</v>
       </c>
+      <c r="DK48" s="14">
+        <f t="shared" si="18"/>
+        <v>3177.3643990403507</v>
+      </c>
+      <c r="DL48" s="14">
+        <f t="shared" si="18"/>
+        <v>-3034.7163748965831</v>
+      </c>
     </row>
-    <row r="49" spans="1:114" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:116" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="20" t="s">
         <v>4</v>
       </c>
@@ -18335,8 +18656,16 @@
         <f t="shared" si="18"/>
         <v>5718.9184383000247</v>
       </c>
+      <c r="DK49" s="23">
+        <f t="shared" si="18"/>
+        <v>7234.1052285998594</v>
+      </c>
+      <c r="DL49" s="23">
+        <f t="shared" si="18"/>
+        <v>-4912.6331431996077</v>
+      </c>
     </row>
-    <row r="50" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>5</v>
       </c>
@@ -18789,8 +19118,16 @@
         <f t="shared" si="18"/>
         <v>-651.41344999999274</v>
       </c>
+      <c r="DK50" s="14">
+        <f t="shared" si="18"/>
+        <v>2180.0335730001098</v>
+      </c>
+      <c r="DL50" s="14">
+        <f t="shared" si="18"/>
+        <v>1171.9063729000045</v>
+      </c>
     </row>
-    <row r="51" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>14</v>
       </c>
@@ -19080,7 +19417,7 @@
         <v>854.40356989996508</v>
       </c>
       <c r="BV51" s="14">
-        <f t="shared" ref="BV51:DJ54" si="21">BV25-BU25</f>
+        <f t="shared" ref="BV51:DL54" si="21">BV25-BU25</f>
         <v>-4001.2403384999488</v>
       </c>
       <c r="BW51" s="14">
@@ -19243,8 +19580,16 @@
         <f t="shared" si="21"/>
         <v>-2366.0644903999637</v>
       </c>
+      <c r="DK51" s="14">
+        <f t="shared" si="21"/>
+        <v>-4007.9991663000546</v>
+      </c>
+      <c r="DL51" s="14">
+        <f t="shared" si="21"/>
+        <v>-1036.1391397999832</v>
+      </c>
     </row>
-    <row r="52" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>13</v>
       </c>
@@ -19697,8 +20042,16 @@
         <f t="shared" si="21"/>
         <v>7533.3975060000084</v>
       </c>
+      <c r="DK52" s="14">
+        <f t="shared" si="21"/>
+        <v>5743.9552761999657</v>
+      </c>
+      <c r="DL52" s="14">
+        <f t="shared" si="21"/>
+        <v>-1278.4824745000224</v>
+      </c>
     </row>
-    <row r="53" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>6</v>
       </c>
@@ -20151,8 +20504,16 @@
         <f t="shared" si="21"/>
         <v>1202.9988726999727</v>
       </c>
+      <c r="DK53" s="14">
+        <f t="shared" si="21"/>
+        <v>3318.1155456998385</v>
+      </c>
+      <c r="DL53" s="14">
+        <f t="shared" si="21"/>
+        <v>-3769.9179017996066</v>
+      </c>
     </row>
-    <row r="54" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>7</v>
       </c>
@@ -20605,8 +20966,16 @@
         <f t="shared" si="21"/>
         <v>1311.4599784000002</v>
       </c>
+      <c r="DK54" s="14">
+        <f t="shared" si="21"/>
+        <v>3954.6387902999995</v>
+      </c>
+      <c r="DL54" s="14">
+        <f t="shared" si="21"/>
+        <v>-4123.7482223999996</v>
+      </c>
     </row>
-    <row r="55" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>8</v>
       </c>
@@ -20740,7 +21109,7 @@
         <v>-36.071311499999865</v>
       </c>
       <c r="AI55" s="14">
-        <f t="shared" ref="AI55:DJ55" si="22">AI29-AH29</f>
+        <f t="shared" ref="AI55:DL55" si="22">AI29-AH29</f>
         <v>-325.20539640000015</v>
       </c>
       <c r="AJ55" s="14">
@@ -21059,21 +21428,29 @@
         <f t="shared" si="22"/>
         <v>-108.46110570000019</v>
       </c>
+      <c r="DK55" s="14">
+        <f t="shared" si="22"/>
+        <v>-636.52324459999977</v>
+      </c>
+      <c r="DL55" s="14">
+        <f t="shared" si="22"/>
+        <v>353.83032060000028</v>
+      </c>
     </row>
-    <row r="56" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A56" s="4"/>
     </row>
-    <row r="57" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A57" s="17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="58" spans="1:114" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:116" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="59" spans="1:114" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:116" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A59" s="17" t="s">
         <v>31</v>
       </c>
@@ -21214,13 +21591,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F896919C-520F-4CD9-9A7E-546D89087BE5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B1062BA-149A-42CB-81E4-00BAE8279A2A}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9C57A6A-8B6F-47DE-B8DB-4C28740745AF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA4A1DAA-A474-4A53-B61F-49323C990B3E}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07FDE7AA-3163-452D-B167-9828AC87734B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1274DFA-5CF2-4681-A908-20ED467E3F84}"/>
 </file>
</xml_diff>

<commit_message>
Auto commit - 2024-06-28
</commit_message>
<xml_diff>
--- a/2024/2024_06_07_CB_loans/2_Money_Base_dayly_eng.xlsx
+++ b/2024/2024_06_07_CB_loans/2_Money_Base_dayly_eng.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBDD3E8A-8335-4ECF-92AB-A311D93B3535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA42D683-8142-4C0A-BFB1-6E301D7371EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="151">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -534,6 +534,30 @@
   </si>
   <si>
     <t>17.06.24</t>
+  </si>
+  <si>
+    <t>18.06.24</t>
+  </si>
+  <si>
+    <t>19.06.24</t>
+  </si>
+  <si>
+    <t>20.06.24</t>
+  </si>
+  <si>
+    <t>21.06.24</t>
+  </si>
+  <si>
+    <t>24.06.24</t>
+  </si>
+  <si>
+    <t>25.06.24</t>
+  </si>
+  <si>
+    <t>26.06.24</t>
+  </si>
+  <si>
+    <t>27.06.24</t>
   </si>
 </sst>
 </file>
@@ -1895,13 +1919,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:DL59"/>
+  <dimension ref="A1:DT59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="DB7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="DK7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="DT26" sqref="DT26"/>
+      <selection pane="bottomRight" activeCell="DY27" sqref="DY27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1917,27 +1941,27 @@
     <col min="65" max="84" width="16" style="7" hidden="1" customWidth="1"/>
     <col min="85" max="85" width="16" style="7" bestFit="1" customWidth="1"/>
     <col min="86" max="104" width="16" style="7" hidden="1" customWidth="1"/>
-    <col min="105" max="116" width="16" style="7" bestFit="1" customWidth="1"/>
-    <col min="117" max="16384" width="11.5703125" style="7"/>
+    <col min="105" max="124" width="16" style="7" bestFit="1" customWidth="1"/>
+    <col min="125" max="16384" width="11.5703125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:116" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:124" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:116" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:124" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:116" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:124" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
     </row>
-    <row r="4" spans="1:116" ht="3" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:124" ht="3" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
     </row>
-    <row r="5" spans="1:116" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:124" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -2286,8 +2310,32 @@
       <c r="DL5" s="10" t="s">
         <v>142</v>
       </c>
+      <c r="DM5" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="DN5" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="DO5" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="DP5" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="DQ5" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="DR5" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="DS5" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="DT5" s="10" t="s">
+        <v>150</v>
+      </c>
     </row>
-    <row r="6" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
@@ -2404,8 +2452,16 @@
       <c r="DJ6" s="12"/>
       <c r="DK6" s="12"/>
       <c r="DL6" s="12"/>
+      <c r="DM6" s="12"/>
+      <c r="DN6" s="12"/>
+      <c r="DO6" s="12"/>
+      <c r="DP6" s="12"/>
+      <c r="DQ6" s="12"/>
+      <c r="DR6" s="12"/>
+      <c r="DS6" s="12"/>
+      <c r="DT6" s="12"/>
     </row>
-    <row r="7" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
@@ -2754,8 +2810,32 @@
       <c r="DL7" s="13">
         <v>939895.1588591066</v>
       </c>
+      <c r="DM7" s="13">
+        <v>954795.02617992356</v>
+      </c>
+      <c r="DN7" s="13">
+        <v>956419.28184687055</v>
+      </c>
+      <c r="DO7" s="13">
+        <v>966732.43608578504</v>
+      </c>
+      <c r="DP7" s="13">
+        <v>966373.04397123051</v>
+      </c>
+      <c r="DQ7" s="13">
+        <v>975177.31295281346</v>
+      </c>
+      <c r="DR7" s="13">
+        <v>974801.49845124444</v>
+      </c>
+      <c r="DS7" s="13">
+        <v>976945.17829130962</v>
+      </c>
+      <c r="DT7" s="13">
+        <v>970176.4741105733</v>
+      </c>
     </row>
-    <row r="8" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
@@ -3104,8 +3184,32 @@
       <c r="DL8" s="13">
         <v>743611.59776629356</v>
       </c>
+      <c r="DM8" s="13">
+        <v>705342.49768877623</v>
+      </c>
+      <c r="DN8" s="13">
+        <v>729980.40096412937</v>
+      </c>
+      <c r="DO8" s="13">
+        <v>672567.9071888146</v>
+      </c>
+      <c r="DP8" s="13">
+        <v>671246.24785276945</v>
+      </c>
+      <c r="DQ8" s="13">
+        <v>677303.55952708633</v>
+      </c>
+      <c r="DR8" s="13">
+        <v>671485.9721679556</v>
+      </c>
+      <c r="DS8" s="13">
+        <v>838967.8725794903</v>
+      </c>
+      <c r="DT8" s="13">
+        <v>852974.48511612648</v>
+      </c>
     </row>
-    <row r="9" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -3454,8 +3558,32 @@
       <c r="DL9" s="13">
         <v>-390767.90789720003</v>
       </c>
+      <c r="DM9" s="13">
+        <v>-409786.4281071999</v>
+      </c>
+      <c r="DN9" s="13">
+        <v>-440771.33079239994</v>
+      </c>
+      <c r="DO9" s="13">
+        <v>-498547.72316450009</v>
+      </c>
+      <c r="DP9" s="13">
+        <v>-502040.73085459997</v>
+      </c>
+      <c r="DQ9" s="13">
+        <v>-496051.24776230002</v>
+      </c>
+      <c r="DR9" s="13">
+        <v>-499008.01314200001</v>
+      </c>
+      <c r="DS9" s="13">
+        <v>-498210.87830889988</v>
+      </c>
+      <c r="DT9" s="13">
+        <v>-494400.26520999998</v>
+      </c>
     </row>
-    <row r="10" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
@@ -3804,8 +3932,32 @@
       <c r="DL10" s="13">
         <v>669332.19195340003</v>
       </c>
+      <c r="DM10" s="13">
+        <v>669462.15864390007</v>
+      </c>
+      <c r="DN10" s="13">
+        <v>705017.76005359995</v>
+      </c>
+      <c r="DO10" s="13">
+        <v>705155.65622469992</v>
+      </c>
+      <c r="DP10" s="13">
+        <v>707468.67480459996</v>
+      </c>
+      <c r="DQ10" s="13">
+        <v>707883.89464669989</v>
+      </c>
+      <c r="DR10" s="13">
+        <v>705052.7840124002</v>
+      </c>
+      <c r="DS10" s="13">
+        <v>881561.02076060011</v>
+      </c>
+      <c r="DT10" s="13">
+        <v>881740.10425810004</v>
+      </c>
     </row>
-    <row r="11" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -4154,8 +4306,32 @@
       <c r="DL11" s="13">
         <v>368410.26691900002</v>
       </c>
+      <c r="DM11" s="13">
+        <v>368492.32030199998</v>
+      </c>
+      <c r="DN11" s="13">
+        <v>404000</v>
+      </c>
+      <c r="DO11" s="13">
+        <v>404089.96605299995</v>
+      </c>
+      <c r="DP11" s="13">
+        <v>404179.93210600002</v>
+      </c>
+      <c r="DQ11" s="13">
+        <v>404449.83026000002</v>
+      </c>
+      <c r="DR11" s="13">
+        <v>404539.79631499999</v>
+      </c>
+      <c r="DS11" s="13">
+        <v>581000</v>
+      </c>
+      <c r="DT11" s="13">
+        <v>581131.04197200004</v>
+      </c>
     </row>
-    <row r="12" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
@@ -4504,8 +4680,32 @@
       <c r="DL12" s="13">
         <v>368410.26691900002</v>
       </c>
+      <c r="DM12" s="13">
+        <v>368492.32030199998</v>
+      </c>
+      <c r="DN12" s="13">
+        <v>404000</v>
+      </c>
+      <c r="DO12" s="13">
+        <v>404089.96605300001</v>
+      </c>
+      <c r="DP12" s="13">
+        <v>404179.93210600002</v>
+      </c>
+      <c r="DQ12" s="13">
+        <v>404449.83026000002</v>
+      </c>
+      <c r="DR12" s="13">
+        <v>404539.79631499999</v>
+      </c>
+      <c r="DS12" s="13">
+        <v>445000</v>
+      </c>
+      <c r="DT12" s="13">
+        <v>445100.96767300001</v>
+      </c>
     </row>
-    <row r="13" spans="1:116" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:124" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -4854,8 +5054,32 @@
       <c r="DL13" s="13">
         <v>0</v>
       </c>
+      <c r="DM13" s="13">
+        <v>0</v>
+      </c>
+      <c r="DN13" s="13">
+        <v>0</v>
+      </c>
+      <c r="DO13" s="13">
+        <v>0</v>
+      </c>
+      <c r="DP13" s="13">
+        <v>0</v>
+      </c>
+      <c r="DQ13" s="13">
+        <v>0</v>
+      </c>
+      <c r="DR13" s="13">
+        <v>0</v>
+      </c>
+      <c r="DS13" s="13">
+        <v>0</v>
+      </c>
+      <c r="DT13" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
@@ -5204,8 +5428,32 @@
       <c r="DL14" s="13">
         <v>0</v>
       </c>
+      <c r="DM14" s="13">
+        <v>0</v>
+      </c>
+      <c r="DN14" s="13">
+        <v>0</v>
+      </c>
+      <c r="DO14" s="13">
+        <v>0</v>
+      </c>
+      <c r="DP14" s="13">
+        <v>0</v>
+      </c>
+      <c r="DQ14" s="13">
+        <v>0</v>
+      </c>
+      <c r="DR14" s="13">
+        <v>0</v>
+      </c>
+      <c r="DS14" s="13">
+        <v>136000</v>
+      </c>
+      <c r="DT14" s="13">
+        <v>136030.074299</v>
+      </c>
     </row>
-    <row r="15" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
@@ -5554,8 +5802,32 @@
       <c r="DL15" s="13">
         <v>0</v>
       </c>
+      <c r="DM15" s="13">
+        <v>0</v>
+      </c>
+      <c r="DN15" s="13">
+        <v>0</v>
+      </c>
+      <c r="DO15" s="13">
+        <v>0</v>
+      </c>
+      <c r="DP15" s="13">
+        <v>0</v>
+      </c>
+      <c r="DQ15" s="13">
+        <v>0</v>
+      </c>
+      <c r="DR15" s="13">
+        <v>0</v>
+      </c>
+      <c r="DS15" s="13">
+        <v>0</v>
+      </c>
+      <c r="DT15" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
@@ -5904,8 +6176,32 @@
       <c r="DL16" s="13">
         <v>0</v>
       </c>
+      <c r="DM16" s="13">
+        <v>0</v>
+      </c>
+      <c r="DN16" s="13">
+        <v>0</v>
+      </c>
+      <c r="DO16" s="13">
+        <v>0</v>
+      </c>
+      <c r="DP16" s="13">
+        <v>0</v>
+      </c>
+      <c r="DQ16" s="13">
+        <v>0</v>
+      </c>
+      <c r="DR16" s="13">
+        <v>0</v>
+      </c>
+      <c r="DS16" s="13">
+        <v>0</v>
+      </c>
+      <c r="DT16" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
@@ -6254,8 +6550,32 @@
       <c r="DL17" s="13">
         <v>0</v>
       </c>
+      <c r="DM17" s="13">
+        <v>0</v>
+      </c>
+      <c r="DN17" s="13">
+        <v>0</v>
+      </c>
+      <c r="DO17" s="13">
+        <v>0</v>
+      </c>
+      <c r="DP17" s="13">
+        <v>0</v>
+      </c>
+      <c r="DQ17" s="13">
+        <v>0</v>
+      </c>
+      <c r="DR17" s="13">
+        <v>0</v>
+      </c>
+      <c r="DS17" s="13">
+        <v>0</v>
+      </c>
+      <c r="DT17" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
@@ -6604,8 +6924,32 @@
       <c r="DL18" s="13">
         <v>0</v>
       </c>
+      <c r="DM18" s="13">
+        <v>0</v>
+      </c>
+      <c r="DN18" s="13">
+        <v>0</v>
+      </c>
+      <c r="DO18" s="13">
+        <v>0</v>
+      </c>
+      <c r="DP18" s="13">
+        <v>0</v>
+      </c>
+      <c r="DQ18" s="13">
+        <v>0</v>
+      </c>
+      <c r="DR18" s="13">
+        <v>0</v>
+      </c>
+      <c r="DS18" s="13">
+        <v>0</v>
+      </c>
+      <c r="DT18" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
@@ -6954,8 +7298,32 @@
       <c r="DL19" s="13">
         <v>0</v>
       </c>
+      <c r="DM19" s="13">
+        <v>0</v>
+      </c>
+      <c r="DN19" s="13">
+        <v>0</v>
+      </c>
+      <c r="DO19" s="13">
+        <v>0</v>
+      </c>
+      <c r="DP19" s="13">
+        <v>0</v>
+      </c>
+      <c r="DQ19" s="13">
+        <v>0</v>
+      </c>
+      <c r="DR19" s="13">
+        <v>0</v>
+      </c>
+      <c r="DS19" s="13">
+        <v>0</v>
+      </c>
+      <c r="DT19" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:116" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:124" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>11</v>
       </c>
@@ -7304,8 +7672,32 @@
       <c r="DL20" s="13">
         <v>0</v>
       </c>
+      <c r="DM20" s="13">
+        <v>0</v>
+      </c>
+      <c r="DN20" s="13">
+        <v>0</v>
+      </c>
+      <c r="DO20" s="13">
+        <v>0</v>
+      </c>
+      <c r="DP20" s="13">
+        <v>0</v>
+      </c>
+      <c r="DQ20" s="13">
+        <v>0</v>
+      </c>
+      <c r="DR20" s="13">
+        <v>0</v>
+      </c>
+      <c r="DS20" s="13">
+        <v>0</v>
+      </c>
+      <c r="DT20" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
@@ -7654,8 +8046,32 @@
       <c r="DL21" s="13">
         <v>0</v>
       </c>
+      <c r="DM21" s="13">
+        <v>0</v>
+      </c>
+      <c r="DN21" s="13">
+        <v>0</v>
+      </c>
+      <c r="DO21" s="13">
+        <v>0</v>
+      </c>
+      <c r="DP21" s="13">
+        <v>0</v>
+      </c>
+      <c r="DQ21" s="13">
+        <v>0</v>
+      </c>
+      <c r="DR21" s="13">
+        <v>0</v>
+      </c>
+      <c r="DS21" s="13">
+        <v>0</v>
+      </c>
+      <c r="DT21" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -8004,8 +8420,32 @@
       <c r="DL22" s="13">
         <v>465047.31371009361</v>
       </c>
+      <c r="DM22" s="13">
+        <v>445666.76715207601</v>
+      </c>
+      <c r="DN22" s="13">
+        <v>465733.97170292935</v>
+      </c>
+      <c r="DO22" s="13">
+        <v>465959.97412861488</v>
+      </c>
+      <c r="DP22" s="13">
+        <v>465818.30390276946</v>
+      </c>
+      <c r="DQ22" s="13">
+        <v>465470.91264268651</v>
+      </c>
+      <c r="DR22" s="13">
+        <v>465441.20129755547</v>
+      </c>
+      <c r="DS22" s="13">
+        <v>455617.73012779013</v>
+      </c>
+      <c r="DT22" s="13">
+        <v>465634.64606802631</v>
+      </c>
     </row>
-    <row r="23" spans="1:116" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:124" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
         <v>4</v>
       </c>
@@ -8354,8 +8794,32 @@
       <c r="DL23" s="21">
         <v>1683506.7566254002</v>
       </c>
+      <c r="DM23" s="21">
+        <v>1660137.5238686998</v>
+      </c>
+      <c r="DN23" s="21">
+        <v>1686399.6828109999</v>
+      </c>
+      <c r="DO23" s="21">
+        <v>1639300.3432745996</v>
+      </c>
+      <c r="DP23" s="21">
+        <v>1637619.291824</v>
+      </c>
+      <c r="DQ23" s="21">
+        <v>1652480.8724798998</v>
+      </c>
+      <c r="DR23" s="21">
+        <v>1646287.4706192</v>
+      </c>
+      <c r="DS23" s="21">
+        <v>1815913.0508707999</v>
+      </c>
+      <c r="DT23" s="21">
+        <v>1823150.9592266998</v>
+      </c>
     </row>
-    <row r="24" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>5</v>
       </c>
@@ -8704,8 +9168,32 @@
       <c r="DL24" s="13">
         <v>890811.5800357</v>
       </c>
+      <c r="DM24" s="13">
+        <v>889505.21595569991</v>
+      </c>
+      <c r="DN24" s="13">
+        <v>887285.49679569993</v>
+      </c>
+      <c r="DO24" s="13">
+        <v>888121.11574569985</v>
+      </c>
+      <c r="DP24" s="13">
+        <v>890145.72412369994</v>
+      </c>
+      <c r="DQ24" s="13">
+        <v>888547.45321249985</v>
+      </c>
+      <c r="DR24" s="13">
+        <v>881286.93105719995</v>
+      </c>
+      <c r="DS24" s="13">
+        <v>880102.09949179995</v>
+      </c>
+      <c r="DT24" s="13">
+        <v>880501.69318079995</v>
+      </c>
     </row>
-    <row r="25" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>14</v>
       </c>
@@ -9054,8 +9542,32 @@
       <c r="DL25" s="13">
         <v>327319.11003029998</v>
       </c>
+      <c r="DM25" s="13">
+        <v>298998.16376730002</v>
+      </c>
+      <c r="DN25" s="13">
+        <v>325198.60219240002</v>
+      </c>
+      <c r="DO25" s="13">
+        <v>279939.28415809997</v>
+      </c>
+      <c r="DP25" s="13">
+        <v>275695.11308570002</v>
+      </c>
+      <c r="DQ25" s="13">
+        <v>272073.1027171</v>
+      </c>
+      <c r="DR25" s="13">
+        <v>293615.6617697</v>
+      </c>
+      <c r="DS25" s="13">
+        <v>472531.34795140004</v>
+      </c>
+      <c r="DT25" s="13">
+        <v>482293.0170004</v>
+      </c>
     </row>
-    <row r="26" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
@@ -9404,8 +9916,32 @@
       <c r="DL26" s="13">
         <v>447558.86425559997</v>
       </c>
+      <c r="DM26" s="13">
+        <v>453547.88766379998</v>
+      </c>
+      <c r="DN26" s="13">
+        <v>454897.70000959997</v>
+      </c>
+      <c r="DO26" s="13">
+        <v>451211.70473489998</v>
+      </c>
+      <c r="DP26" s="13">
+        <v>451066.446268</v>
+      </c>
+      <c r="DQ26" s="13">
+        <v>451268.64494090003</v>
+      </c>
+      <c r="DR26" s="13">
+        <v>445418.03647970001</v>
+      </c>
+      <c r="DS26" s="13">
+        <v>443186.99594270001</v>
+      </c>
+      <c r="DT26" s="13">
+        <v>441666.94042449998</v>
+      </c>
     </row>
-    <row r="27" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>6</v>
       </c>
@@ -9754,8 +10290,32 @@
       <c r="DL27" s="13">
         <v>17817.202303800208</v>
       </c>
+      <c r="DM27" s="13">
+        <v>18086.25648189988</v>
+      </c>
+      <c r="DN27" s="13">
+        <v>19017.883813299995</v>
+      </c>
+      <c r="DO27" s="13">
+        <v>20028.238635899848</v>
+      </c>
+      <c r="DP27" s="13">
+        <v>20712.008346599992</v>
+      </c>
+      <c r="DQ27" s="13">
+        <v>40591.671609399898</v>
+      </c>
+      <c r="DR27" s="13">
+        <v>25966.841312600067</v>
+      </c>
+      <c r="DS27" s="13">
+        <v>20092.607484899927</v>
+      </c>
+      <c r="DT27" s="13">
+        <v>18689.308620999858</v>
+      </c>
     </row>
-    <row r="28" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>7</v>
       </c>
@@ -10104,8 +10664,32 @@
       <c r="DL28" s="13">
         <v>15441.157375000001</v>
       </c>
+      <c r="DM28" s="13">
+        <v>15355.6944245</v>
+      </c>
+      <c r="DN28" s="13">
+        <v>16291.7885475</v>
+      </c>
+      <c r="DO28" s="13">
+        <v>18063.861337000002</v>
+      </c>
+      <c r="DP28" s="13">
+        <v>17087.6359854</v>
+      </c>
+      <c r="DQ28" s="13">
+        <v>29351.867085099999</v>
+      </c>
+      <c r="DR28" s="13">
+        <v>22679.536457800001</v>
+      </c>
+      <c r="DS28" s="13">
+        <v>15663.4967557</v>
+      </c>
+      <c r="DT28" s="13">
+        <v>15833.7303235</v>
+      </c>
     </row>
-    <row r="29" spans="1:116" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:124" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -10454,8 +11038,32 @@
       <c r="DL29" s="13">
         <v>2376.0449288000004</v>
       </c>
+      <c r="DM29" s="13">
+        <v>2730.5620574000004</v>
+      </c>
+      <c r="DN29" s="13">
+        <v>2726.0952658000001</v>
+      </c>
+      <c r="DO29" s="13">
+        <v>1964.3772989000001</v>
+      </c>
+      <c r="DP29" s="13">
+        <v>3624.3723611999999</v>
+      </c>
+      <c r="DQ29" s="13">
+        <v>11239.8045243</v>
+      </c>
+      <c r="DR29" s="13">
+        <v>3287.3048548000002</v>
+      </c>
+      <c r="DS29" s="13">
+        <v>4429.1107291999997</v>
+      </c>
+      <c r="DT29" s="13">
+        <v>2855.5782974999997</v>
+      </c>
     </row>
-    <row r="30" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
@@ -10572,8 +11180,16 @@
       <c r="DJ30" s="14"/>
       <c r="DK30" s="14"/>
       <c r="DL30" s="14"/>
+      <c r="DM30" s="14"/>
+      <c r="DN30" s="14"/>
+      <c r="DO30" s="14"/>
+      <c r="DP30" s="14"/>
+      <c r="DQ30" s="14"/>
+      <c r="DR30" s="14"/>
+      <c r="DS30" s="14"/>
+      <c r="DT30" s="14"/>
     </row>
-    <row r="31" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>15</v>
       </c>
@@ -10692,8 +11308,16 @@
       <c r="DJ31" s="15"/>
       <c r="DK31" s="15"/>
       <c r="DL31" s="15"/>
+      <c r="DM31" s="15"/>
+      <c r="DN31" s="15"/>
+      <c r="DO31" s="15"/>
+      <c r="DP31" s="15"/>
+      <c r="DQ31" s="15"/>
+      <c r="DR31" s="15"/>
+      <c r="DS31" s="15"/>
+      <c r="DT31" s="15"/>
     </row>
-    <row r="32" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
@@ -10810,8 +11434,16 @@
       <c r="DJ32" s="16"/>
       <c r="DK32" s="16"/>
       <c r="DL32" s="16"/>
+      <c r="DM32" s="16"/>
+      <c r="DN32" s="16"/>
+      <c r="DO32" s="16"/>
+      <c r="DP32" s="16"/>
+      <c r="DQ32" s="16"/>
+      <c r="DR32" s="16"/>
+      <c r="DS32" s="16"/>
+      <c r="DT32" s="16"/>
     </row>
-    <row r="33" spans="1:116" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:124" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>19</v>
       </c>
@@ -11137,7 +11769,7 @@
         <v>-7222.5502792990301</v>
       </c>
       <c r="CE33" s="14">
-        <f t="shared" ref="CE33:DL37" si="5">CE7-CD7</f>
+        <f t="shared" ref="CE33:DT37" si="5">CE7-CD7</f>
         <v>-2284.7872705847258</v>
       </c>
       <c r="CF33" s="14">
@@ -11272,8 +11904,40 @@
         <f t="shared" si="5"/>
         <v>-2605.4993798030773</v>
       </c>
+      <c r="DM33" s="14">
+        <f t="shared" si="5"/>
+        <v>14899.867320816964</v>
+      </c>
+      <c r="DN33" s="14">
+        <f t="shared" si="5"/>
+        <v>1624.2556669469923</v>
+      </c>
+      <c r="DO33" s="14">
+        <f t="shared" si="5"/>
+        <v>10313.154238914489</v>
+      </c>
+      <c r="DP33" s="14">
+        <f t="shared" si="5"/>
+        <v>-359.39211455453187</v>
+      </c>
+      <c r="DQ33" s="14">
+        <f t="shared" si="5"/>
+        <v>8804.2689815829508</v>
+      </c>
+      <c r="DR33" s="14">
+        <f t="shared" si="5"/>
+        <v>-375.81450156902429</v>
+      </c>
+      <c r="DS33" s="14">
+        <f t="shared" si="5"/>
+        <v>2143.6798400651896</v>
+      </c>
+      <c r="DT33" s="14">
+        <f t="shared" si="5"/>
+        <v>-6768.7041807363275</v>
+      </c>
     </row>
-    <row r="34" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>22</v>
       </c>
@@ -11734,8 +12398,40 @@
         <f t="shared" si="5"/>
         <v>-2307.1337633965304</v>
       </c>
+      <c r="DM34" s="14">
+        <f t="shared" si="5"/>
+        <v>-38269.100077517331</v>
+      </c>
+      <c r="DN34" s="14">
+        <f t="shared" si="5"/>
+        <v>24637.903275353136</v>
+      </c>
+      <c r="DO34" s="14">
+        <f t="shared" si="5"/>
+        <v>-57412.493775314768</v>
+      </c>
+      <c r="DP34" s="14">
+        <f t="shared" si="5"/>
+        <v>-1321.6593360451516</v>
+      </c>
+      <c r="DQ34" s="14">
+        <f t="shared" si="5"/>
+        <v>6057.3116743168794</v>
+      </c>
+      <c r="DR34" s="14">
+        <f t="shared" si="5"/>
+        <v>-5817.5873591307318</v>
+      </c>
+      <c r="DS34" s="14">
+        <f t="shared" si="5"/>
+        <v>167481.90041153471</v>
+      </c>
+      <c r="DT34" s="14">
+        <f t="shared" si="5"/>
+        <v>14006.612536636181</v>
+      </c>
     </row>
-    <row r="35" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>2</v>
       </c>
@@ -12196,8 +12892,40 @@
         <f t="shared" si="5"/>
         <v>1690.9172753999592</v>
       </c>
+      <c r="DM35" s="14">
+        <f t="shared" si="5"/>
+        <v>-19018.520209999871</v>
+      </c>
+      <c r="DN35" s="14">
+        <f t="shared" si="5"/>
+        <v>-30984.902685200039</v>
+      </c>
+      <c r="DO35" s="14">
+        <f t="shared" si="5"/>
+        <v>-57776.392372100148</v>
+      </c>
+      <c r="DP35" s="14">
+        <f t="shared" si="5"/>
+        <v>-3493.0076900998829</v>
+      </c>
+      <c r="DQ35" s="14">
+        <f t="shared" si="5"/>
+        <v>5989.4830922999536</v>
+      </c>
+      <c r="DR35" s="14">
+        <f t="shared" si="5"/>
+        <v>-2956.7653796999948</v>
+      </c>
+      <c r="DS35" s="14">
+        <f t="shared" si="5"/>
+        <v>797.13483310013544</v>
+      </c>
+      <c r="DT35" s="14">
+        <f t="shared" si="5"/>
+        <v>3810.6130988998921</v>
+      </c>
     </row>
-    <row r="36" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>3</v>
       </c>
@@ -12658,8 +13386,40 @@
         <f t="shared" si="5"/>
         <v>-963.33466389996465</v>
       </c>
+      <c r="DM36" s="14">
+        <f t="shared" si="5"/>
+        <v>129.96669050003402</v>
+      </c>
+      <c r="DN36" s="14">
+        <f t="shared" si="5"/>
+        <v>35555.601409699884</v>
+      </c>
+      <c r="DO36" s="14">
+        <f t="shared" si="5"/>
+        <v>137.89617109997198</v>
+      </c>
+      <c r="DP36" s="14">
+        <f t="shared" si="5"/>
+        <v>2313.0185799000319</v>
+      </c>
+      <c r="DQ36" s="14">
+        <f t="shared" si="5"/>
+        <v>415.21984209993389</v>
+      </c>
+      <c r="DR36" s="14">
+        <f t="shared" si="5"/>
+        <v>-2831.1106342996936</v>
+      </c>
+      <c r="DS36" s="14">
+        <f t="shared" si="5"/>
+        <v>176508.23674819991</v>
+      </c>
+      <c r="DT36" s="14">
+        <f t="shared" si="5"/>
+        <v>179.08349749993067</v>
+      </c>
     </row>
-    <row r="37" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>17</v>
       </c>
@@ -13120,8 +13880,40 @@
         <f t="shared" si="5"/>
         <v>246.16015100001823</v>
       </c>
+      <c r="DM37" s="14">
+        <f t="shared" si="5"/>
+        <v>82.053382999962196</v>
+      </c>
+      <c r="DN37" s="14">
+        <f t="shared" si="5"/>
+        <v>35507.679698000022</v>
+      </c>
+      <c r="DO37" s="14">
+        <f t="shared" si="5"/>
+        <v>89.966052999952808</v>
+      </c>
+      <c r="DP37" s="14">
+        <f t="shared" si="5"/>
+        <v>89.966053000069223</v>
+      </c>
+      <c r="DQ37" s="14">
+        <f t="shared" si="5"/>
+        <v>269.89815399999497</v>
+      </c>
+      <c r="DR37" s="14">
+        <f t="shared" si="5"/>
+        <v>89.966054999968037</v>
+      </c>
+      <c r="DS37" s="14">
+        <f t="shared" si="5"/>
+        <v>176460.20368500001</v>
+      </c>
+      <c r="DT37" s="14">
+        <f t="shared" si="5"/>
+        <v>131.04197200003546</v>
+      </c>
     </row>
-    <row r="38" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>23</v>
       </c>
@@ -13443,7 +14235,7 @@
         <v>92.435473999998067</v>
       </c>
       <c r="CD38" s="14">
-        <f t="shared" ref="CD38:DL42" si="9">CD12-CC12</f>
+        <f t="shared" ref="CD38:DT42" si="9">CD12-CC12</f>
         <v>84445.387153999996</v>
       </c>
       <c r="CE38" s="14">
@@ -13582,8 +14374,40 @@
         <f t="shared" si="9"/>
         <v>246.16015100001823</v>
       </c>
+      <c r="DM38" s="14">
+        <f t="shared" si="9"/>
+        <v>82.053382999962196</v>
+      </c>
+      <c r="DN38" s="14">
+        <f t="shared" si="9"/>
+        <v>35507.679698000022</v>
+      </c>
+      <c r="DO38" s="14">
+        <f t="shared" si="9"/>
+        <v>89.966053000011016</v>
+      </c>
+      <c r="DP38" s="14">
+        <f t="shared" si="9"/>
+        <v>89.966053000011016</v>
+      </c>
+      <c r="DQ38" s="14">
+        <f t="shared" si="9"/>
+        <v>269.89815399999497</v>
+      </c>
+      <c r="DR38" s="14">
+        <f t="shared" si="9"/>
+        <v>89.966054999968037</v>
+      </c>
+      <c r="DS38" s="14">
+        <f t="shared" si="9"/>
+        <v>40460.203685000015</v>
+      </c>
+      <c r="DT38" s="14">
+        <f t="shared" si="9"/>
+        <v>100.96767300000647</v>
+      </c>
     </row>
-    <row r="39" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>24</v>
       </c>
@@ -14044,8 +14868,40 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="DM39" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DN39" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DO39" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DP39" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DQ39" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DR39" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DS39" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DT39" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="40" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>25</v>
       </c>
@@ -14506,8 +15362,40 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="DM40" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DN40" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DO40" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DP40" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DQ40" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DR40" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DS40" s="14">
+        <f t="shared" si="9"/>
+        <v>136000</v>
+      </c>
+      <c r="DT40" s="14">
+        <f t="shared" si="9"/>
+        <v>30.074298999999883</v>
+      </c>
     </row>
-    <row r="41" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>26</v>
       </c>
@@ -14968,8 +15856,40 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="DM41" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DN41" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DO41" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DP41" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DQ41" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DR41" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DS41" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DT41" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="42" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>9</v>
       </c>
@@ -15430,8 +16350,40 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="DM42" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DN42" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DO42" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DP42" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DQ42" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DR42" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DS42" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="DT42" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="43" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>10</v>
       </c>
@@ -15865,7 +16817,7 @@
         <v>0</v>
       </c>
       <c r="DF43" s="14">
-        <f t="shared" ref="DF43:DL47" si="12">-(DF17-DE17)</f>
+        <f t="shared" ref="DF43:DT47" si="12">-(DF17-DE17)</f>
         <v>17003.135245900001</v>
       </c>
       <c r="DG43" s="14">
@@ -15892,8 +16844,40 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
+      <c r="DM43" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DN43" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DO43" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DP43" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DQ43" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DR43" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DS43" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DT43" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="44" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>12</v>
       </c>
@@ -16354,8 +17338,40 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
+      <c r="DM44" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DN44" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DO44" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DP44" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DQ44" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DR44" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DS44" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DT44" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="45" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>18</v>
       </c>
@@ -16816,8 +17832,40 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
+      <c r="DM45" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DN45" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DO45" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DP45" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DQ45" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DR45" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DS45" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DT45" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="46" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>11</v>
       </c>
@@ -17278,8 +18326,40 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
+      <c r="DM46" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DN46" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DO46" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DP46" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DQ46" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DR46" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DS46" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DT46" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="47" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>16</v>
       </c>
@@ -17740,8 +18820,40 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
+      <c r="DM47" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DN47" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DO47" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DP47" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DQ47" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DR47" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DS47" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="DT47" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>21</v>
       </c>
@@ -18035,7 +19147,7 @@
         <v>-3678.5371843058383</v>
       </c>
       <c r="BW48" s="14">
-        <f t="shared" ref="BW48:DL50" si="18">BW22-BV22</f>
+        <f t="shared" ref="BW48:DT50" si="18">BW22-BV22</f>
         <v>-4079.5047014922602</v>
       </c>
       <c r="BX48" s="14">
@@ -18202,8 +19314,40 @@
         <f t="shared" si="18"/>
         <v>-3034.7163748965831</v>
       </c>
+      <c r="DM48" s="14">
+        <f t="shared" si="18"/>
+        <v>-19380.54655801761</v>
+      </c>
+      <c r="DN48" s="14">
+        <f t="shared" si="18"/>
+        <v>20067.204550853348</v>
+      </c>
+      <c r="DO48" s="14">
+        <f t="shared" si="18"/>
+        <v>226.00242568552494</v>
+      </c>
+      <c r="DP48" s="14">
+        <f t="shared" si="18"/>
+        <v>-141.67022584541701</v>
+      </c>
+      <c r="DQ48" s="14">
+        <f t="shared" si="18"/>
+        <v>-347.39126008294988</v>
+      </c>
+      <c r="DR48" s="14">
+        <f t="shared" si="18"/>
+        <v>-29.711345131043345</v>
+      </c>
+      <c r="DS48" s="14">
+        <f t="shared" si="18"/>
+        <v>-9823.4711697653402</v>
+      </c>
+      <c r="DT48" s="14">
+        <f t="shared" si="18"/>
+        <v>10016.915940236184</v>
+      </c>
     </row>
-    <row r="49" spans="1:116" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:124" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="20" t="s">
         <v>4</v>
       </c>
@@ -18664,8 +19808,40 @@
         <f t="shared" si="18"/>
         <v>-4912.6331431996077</v>
       </c>
+      <c r="DM49" s="23">
+        <f t="shared" si="18"/>
+        <v>-23369.232756700367</v>
+      </c>
+      <c r="DN49" s="23">
+        <f t="shared" si="18"/>
+        <v>26262.158942300128</v>
+      </c>
+      <c r="DO49" s="23">
+        <f t="shared" si="18"/>
+        <v>-47099.339536400279</v>
+      </c>
+      <c r="DP49" s="23">
+        <f t="shared" si="18"/>
+        <v>-1681.0514505996834</v>
+      </c>
+      <c r="DQ49" s="23">
+        <f t="shared" si="18"/>
+        <v>14861.58065589983</v>
+      </c>
+      <c r="DR49" s="23">
+        <f t="shared" si="18"/>
+        <v>-6193.4018606997561</v>
+      </c>
+      <c r="DS49" s="23">
+        <f t="shared" si="18"/>
+        <v>169625.58025159989</v>
+      </c>
+      <c r="DT49" s="23">
+        <f t="shared" si="18"/>
+        <v>7237.9083558998536</v>
+      </c>
     </row>
-    <row r="50" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>5</v>
       </c>
@@ -19126,8 +20302,40 @@
         <f t="shared" si="18"/>
         <v>1171.9063729000045</v>
       </c>
+      <c r="DM50" s="14">
+        <f t="shared" si="18"/>
+        <v>-1306.3640800000867</v>
+      </c>
+      <c r="DN50" s="14">
+        <f t="shared" si="18"/>
+        <v>-2219.7191599999787</v>
+      </c>
+      <c r="DO50" s="14">
+        <f t="shared" si="18"/>
+        <v>835.61894999991637</v>
+      </c>
+      <c r="DP50" s="14">
+        <f t="shared" si="18"/>
+        <v>2024.6083780000918</v>
+      </c>
+      <c r="DQ50" s="14">
+        <f t="shared" si="18"/>
+        <v>-1598.2709112000884</v>
+      </c>
+      <c r="DR50" s="14">
+        <f t="shared" si="18"/>
+        <v>-7260.5221552998992</v>
+      </c>
+      <c r="DS50" s="14">
+        <f t="shared" si="18"/>
+        <v>-1184.8315654000035</v>
+      </c>
+      <c r="DT50" s="14">
+        <f t="shared" si="18"/>
+        <v>399.59368900000118</v>
+      </c>
     </row>
-    <row r="51" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>14</v>
       </c>
@@ -19417,7 +20625,7 @@
         <v>854.40356989996508</v>
       </c>
       <c r="BV51" s="14">
-        <f t="shared" ref="BV51:DL54" si="21">BV25-BU25</f>
+        <f t="shared" ref="BV51:DT54" si="21">BV25-BU25</f>
         <v>-4001.2403384999488</v>
       </c>
       <c r="BW51" s="14">
@@ -19588,8 +20796,40 @@
         <f t="shared" si="21"/>
         <v>-1036.1391397999832</v>
       </c>
+      <c r="DM51" s="14">
+        <f t="shared" si="21"/>
+        <v>-28320.946262999962</v>
+      </c>
+      <c r="DN51" s="14">
+        <f t="shared" si="21"/>
+        <v>26200.438425100001</v>
+      </c>
+      <c r="DO51" s="14">
+        <f t="shared" si="21"/>
+        <v>-45259.318034300057</v>
+      </c>
+      <c r="DP51" s="14">
+        <f t="shared" si="21"/>
+        <v>-4244.1710723999422</v>
+      </c>
+      <c r="DQ51" s="14">
+        <f t="shared" si="21"/>
+        <v>-3622.010368600022</v>
+      </c>
+      <c r="DR51" s="14">
+        <f t="shared" si="21"/>
+        <v>21542.559052600001</v>
+      </c>
+      <c r="DS51" s="14">
+        <f t="shared" si="21"/>
+        <v>178915.68618170003</v>
+      </c>
+      <c r="DT51" s="14">
+        <f t="shared" si="21"/>
+        <v>9761.6690489999601</v>
+      </c>
     </row>
-    <row r="52" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>13</v>
       </c>
@@ -20050,8 +21290,40 @@
         <f t="shared" si="21"/>
         <v>-1278.4824745000224</v>
       </c>
+      <c r="DM52" s="14">
+        <f t="shared" si="21"/>
+        <v>5989.0234082000097</v>
+      </c>
+      <c r="DN52" s="14">
+        <f t="shared" si="21"/>
+        <v>1349.81234579999</v>
+      </c>
+      <c r="DO52" s="14">
+        <f t="shared" si="21"/>
+        <v>-3685.9952746999916</v>
+      </c>
+      <c r="DP52" s="14">
+        <f t="shared" si="21"/>
+        <v>-145.25846689997707</v>
+      </c>
+      <c r="DQ52" s="14">
+        <f t="shared" si="21"/>
+        <v>202.19867290003458</v>
+      </c>
+      <c r="DR52" s="14">
+        <f t="shared" si="21"/>
+        <v>-5850.6084612000268</v>
+      </c>
+      <c r="DS52" s="14">
+        <f t="shared" si="21"/>
+        <v>-2231.0405369999935</v>
+      </c>
+      <c r="DT52" s="14">
+        <f t="shared" si="21"/>
+        <v>-1520.0555182000389</v>
+      </c>
     </row>
-    <row r="53" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>6</v>
       </c>
@@ -20512,8 +21784,40 @@
         <f t="shared" si="21"/>
         <v>-3769.9179017996066</v>
       </c>
+      <c r="DM53" s="14">
+        <f t="shared" si="21"/>
+        <v>269.05417809967184</v>
+      </c>
+      <c r="DN53" s="14">
+        <f t="shared" si="21"/>
+        <v>931.62733140011551</v>
+      </c>
+      <c r="DO53" s="14">
+        <f t="shared" si="21"/>
+        <v>1010.3548225998529</v>
+      </c>
+      <c r="DP53" s="14">
+        <f t="shared" si="21"/>
+        <v>683.76971070014406</v>
+      </c>
+      <c r="DQ53" s="14">
+        <f t="shared" si="21"/>
+        <v>19879.663262799906</v>
+      </c>
+      <c r="DR53" s="14">
+        <f t="shared" si="21"/>
+        <v>-14624.830296799832</v>
+      </c>
+      <c r="DS53" s="14">
+        <f t="shared" si="21"/>
+        <v>-5874.23382770014</v>
+      </c>
+      <c r="DT53" s="14">
+        <f t="shared" si="21"/>
+        <v>-1403.2988639000687</v>
+      </c>
     </row>
-    <row r="54" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>7</v>
       </c>
@@ -20974,8 +22278,40 @@
         <f t="shared" si="21"/>
         <v>-4123.7482223999996</v>
       </c>
+      <c r="DM54" s="14">
+        <f t="shared" si="21"/>
+        <v>-85.46295050000117</v>
+      </c>
+      <c r="DN54" s="14">
+        <f t="shared" si="21"/>
+        <v>936.09412300000076</v>
+      </c>
+      <c r="DO54" s="14">
+        <f t="shared" si="21"/>
+        <v>1772.0727895000018</v>
+      </c>
+      <c r="DP54" s="14">
+        <f t="shared" si="21"/>
+        <v>-976.22535160000189</v>
+      </c>
+      <c r="DQ54" s="14">
+        <f t="shared" si="21"/>
+        <v>12264.231099699999</v>
+      </c>
+      <c r="DR54" s="14">
+        <f t="shared" si="21"/>
+        <v>-6672.330627299998</v>
+      </c>
+      <c r="DS54" s="14">
+        <f t="shared" si="21"/>
+        <v>-7016.0397021000008</v>
+      </c>
+      <c r="DT54" s="14">
+        <f t="shared" si="21"/>
+        <v>170.23356779999995</v>
+      </c>
     </row>
-    <row r="55" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>8</v>
       </c>
@@ -21109,7 +22445,7 @@
         <v>-36.071311499999865</v>
       </c>
       <c r="AI55" s="14">
-        <f t="shared" ref="AI55:DL55" si="22">AI29-AH29</f>
+        <f t="shared" ref="AI55:DT55" si="22">AI29-AH29</f>
         <v>-325.20539640000015</v>
       </c>
       <c r="AJ55" s="14">
@@ -21436,21 +22772,53 @@
         <f t="shared" si="22"/>
         <v>353.83032060000028</v>
       </c>
+      <c r="DM55" s="14">
+        <f t="shared" si="22"/>
+        <v>354.51712859999998</v>
+      </c>
+      <c r="DN55" s="14">
+        <f t="shared" si="22"/>
+        <v>-4.4667916000003061</v>
+      </c>
+      <c r="DO55" s="14">
+        <f t="shared" si="22"/>
+        <v>-761.71796689999996</v>
+      </c>
+      <c r="DP55" s="14">
+        <f t="shared" si="22"/>
+        <v>1659.9950622999997</v>
+      </c>
+      <c r="DQ55" s="14">
+        <f t="shared" si="22"/>
+        <v>7615.4321631000003</v>
+      </c>
+      <c r="DR55" s="14">
+        <f t="shared" si="22"/>
+        <v>-7952.4996694999991</v>
+      </c>
+      <c r="DS55" s="14">
+        <f t="shared" si="22"/>
+        <v>1141.8058743999995</v>
+      </c>
+      <c r="DT55" s="14">
+        <f t="shared" si="22"/>
+        <v>-1573.5324317</v>
+      </c>
     </row>
-    <row r="56" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A56" s="4"/>
     </row>
-    <row r="57" spans="1:116" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A57" s="17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="58" spans="1:116" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:124" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="59" spans="1:116" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:124" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A59" s="17" t="s">
         <v>31</v>
       </c>
@@ -21591,13 +22959,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B1062BA-149A-42CB-81E4-00BAE8279A2A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D56644F-7B68-45D2-AB56-F75FD0F36712}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA4A1DAA-A474-4A53-B61F-49323C990B3E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAED9A26-45FD-45BB-BE0F-39F6AAF47FEF}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1274DFA-5CF2-4681-A908-20ED467E3F84}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7903EC78-0DA4-4660-98BB-6AA1CCD76CE9}"/>
 </file>
</xml_diff>

<commit_message>
Auto commit - 2024-08-09
</commit_message>
<xml_diff>
--- a/2024/2024_06_07_CB_loans/2_Money_Base_dayly_eng.xlsx
+++ b/2024/2024_06_07_CB_loans/2_Money_Base_dayly_eng.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7585DAE4-0DB9-42EF-A57D-CEDF9BA25B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00944ECB-4651-4880-9325-F6F709D7D9CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="177">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -627,6 +627,15 @@
   </si>
   <si>
     <t>02.08.24</t>
+  </si>
+  <si>
+    <t>05.08.24</t>
+  </si>
+  <si>
+    <t>06.08.24</t>
+  </si>
+  <si>
+    <t>07.08.2024</t>
   </si>
 </sst>
 </file>
@@ -1988,13 +1997,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:ES59"/>
+  <dimension ref="A1:EV59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="DU7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="FF26" sqref="FF26"/>
+      <selection pane="bottomRight" activeCell="FC30" sqref="FC30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2014,27 +2023,27 @@
     <col min="106" max="124" width="16" style="7" hidden="1" customWidth="1"/>
     <col min="125" max="125" width="16" style="7" bestFit="1" customWidth="1"/>
     <col min="126" max="146" width="16" style="7" hidden="1" customWidth="1"/>
-    <col min="147" max="149" width="16" style="7" bestFit="1" customWidth="1"/>
-    <col min="150" max="16384" width="11.5703125" style="7"/>
+    <col min="147" max="152" width="16" style="7" bestFit="1" customWidth="1"/>
+    <col min="153" max="16384" width="11.5703125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:149" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:152" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:149" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:152" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:149" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:152" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
     </row>
-    <row r="4" spans="1:149" ht="3" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:152" ht="3" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
     </row>
-    <row r="5" spans="1:149" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:152" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -2482,8 +2491,17 @@
       <c r="ES5" s="10" t="s">
         <v>173</v>
       </c>
+      <c r="ET5" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="EU5" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="EV5" s="10" t="s">
+        <v>176</v>
+      </c>
     </row>
-    <row r="6" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
@@ -2633,8 +2651,11 @@
       <c r="EQ6" s="12"/>
       <c r="ER6" s="12"/>
       <c r="ES6" s="12"/>
+      <c r="ET6" s="12"/>
+      <c r="EU6" s="12"/>
+      <c r="EV6" s="12"/>
     </row>
-    <row r="7" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
@@ -3082,8 +3103,17 @@
       <c r="ES7" s="13">
         <v>1010006.0205808171</v>
       </c>
+      <c r="ET7" s="13">
+        <v>1019903.1567539917</v>
+      </c>
+      <c r="EU7" s="13">
+        <v>1022256.462715619</v>
+      </c>
+      <c r="EV7" s="13">
+        <v>1043300.1587099641</v>
+      </c>
     </row>
-    <row r="8" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
@@ -3531,8 +3561,17 @@
       <c r="ES8" s="13">
         <v>713871.76782198309</v>
       </c>
+      <c r="ET8" s="13">
+        <v>729931.27807690832</v>
+      </c>
+      <c r="EU8" s="13">
+        <v>728164.86264718091</v>
+      </c>
+      <c r="EV8" s="13">
+        <v>690039.13689563575</v>
+      </c>
     </row>
-    <row r="9" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -3980,8 +4019,17 @@
       <c r="ES9" s="13">
         <v>-455248.66974880005</v>
       </c>
+      <c r="ET9" s="13">
+        <v>-431460.58283209999</v>
+      </c>
+      <c r="EU9" s="13">
+        <v>-434607.37302579993</v>
+      </c>
+      <c r="EV9" s="13">
+        <v>-435134.87206989998</v>
+      </c>
     </row>
-    <row r="10" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
@@ -4429,8 +4477,17 @@
       <c r="ES10" s="13">
         <v>714437.94899840001</v>
       </c>
+      <c r="ET10" s="13">
+        <v>714850.71336109994</v>
+      </c>
+      <c r="EU10" s="13">
+        <v>715330.64265149995</v>
+      </c>
+      <c r="EV10" s="13">
+        <v>676846.61337290006</v>
+      </c>
     </row>
-    <row r="11" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -4878,8 +4935,17 @@
       <c r="ES11" s="13">
         <v>410177.48576800001</v>
       </c>
+      <c r="ET11" s="13">
+        <v>410443.71442600002</v>
+      </c>
+      <c r="EU11" s="13">
+        <v>410532.45731099998</v>
+      </c>
+      <c r="EV11" s="13">
+        <v>375000</v>
+      </c>
     </row>
-    <row r="12" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
@@ -5327,8 +5393,17 @@
       <c r="ES12" s="13">
         <v>410177.48576800001</v>
       </c>
+      <c r="ET12" s="13">
+        <v>410443.71442600002</v>
+      </c>
+      <c r="EU12" s="13">
+        <v>410532.45731099998</v>
+      </c>
+      <c r="EV12" s="13">
+        <v>375000</v>
+      </c>
     </row>
-    <row r="13" spans="1:149" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:152" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -5776,8 +5851,17 @@
       <c r="ES13" s="13">
         <v>0</v>
       </c>
+      <c r="ET13" s="13">
+        <v>0</v>
+      </c>
+      <c r="EU13" s="13">
+        <v>0</v>
+      </c>
+      <c r="EV13" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
@@ -6225,8 +6309,17 @@
       <c r="ES14" s="13">
         <v>0</v>
       </c>
+      <c r="ET14" s="13">
+        <v>0</v>
+      </c>
+      <c r="EU14" s="13">
+        <v>0</v>
+      </c>
+      <c r="EV14" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
@@ -6674,8 +6767,17 @@
       <c r="ES15" s="13">
         <v>0</v>
       </c>
+      <c r="ET15" s="13">
+        <v>0</v>
+      </c>
+      <c r="EU15" s="13">
+        <v>0</v>
+      </c>
+      <c r="EV15" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
@@ -7123,8 +7225,17 @@
       <c r="ES16" s="13">
         <v>0</v>
       </c>
+      <c r="ET16" s="13">
+        <v>0</v>
+      </c>
+      <c r="EU16" s="13">
+        <v>0</v>
+      </c>
+      <c r="EV16" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
@@ -7572,8 +7683,17 @@
       <c r="ES17" s="13">
         <v>0</v>
       </c>
+      <c r="ET17" s="13">
+        <v>0</v>
+      </c>
+      <c r="EU17" s="13">
+        <v>0</v>
+      </c>
+      <c r="EV17" s="13">
+        <v>-3000.5122951000003</v>
+      </c>
     </row>
-    <row r="18" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
@@ -8021,8 +8141,17 @@
       <c r="ES18" s="13">
         <v>0</v>
       </c>
+      <c r="ET18" s="13">
+        <v>0</v>
+      </c>
+      <c r="EU18" s="13">
+        <v>0</v>
+      </c>
+      <c r="EV18" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
@@ -8470,8 +8599,17 @@
       <c r="ES19" s="13">
         <v>0</v>
       </c>
+      <c r="ET19" s="13">
+        <v>0</v>
+      </c>
+      <c r="EU19" s="13">
+        <v>0</v>
+      </c>
+      <c r="EV19" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:149" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:152" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>11</v>
       </c>
@@ -8919,8 +9057,17 @@
       <c r="ES20" s="13">
         <v>0</v>
       </c>
+      <c r="ET20" s="13">
+        <v>0</v>
+      </c>
+      <c r="EU20" s="13">
+        <v>0</v>
+      </c>
+      <c r="EV20" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
@@ -9368,8 +9515,17 @@
       <c r="ES21" s="13">
         <v>0</v>
       </c>
+      <c r="ET21" s="13">
+        <v>0</v>
+      </c>
+      <c r="EU21" s="13">
+        <v>0</v>
+      </c>
+      <c r="EV21" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -9817,8 +9973,17 @@
       <c r="ES22" s="13">
         <v>454682.48857238307</v>
       </c>
+      <c r="ET22" s="13">
+        <v>446541.14754790848</v>
+      </c>
+      <c r="EU22" s="13">
+        <v>447441.59302148083</v>
+      </c>
+      <c r="EV22" s="13">
+        <v>448327.39559263573</v>
+      </c>
     </row>
-    <row r="23" spans="1:149" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:152" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
         <v>4</v>
       </c>
@@ -10266,8 +10431,17 @@
       <c r="ES23" s="21">
         <v>1723877.7884028002</v>
       </c>
+      <c r="ET23" s="21">
+        <v>1749834.4348309</v>
+      </c>
+      <c r="EU23" s="21">
+        <v>1750421.3253627999</v>
+      </c>
+      <c r="EV23" s="21">
+        <v>1733339.2956055999</v>
+      </c>
     </row>
-    <row r="24" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>5</v>
       </c>
@@ -10715,8 +10889,17 @@
       <c r="ES24" s="13">
         <v>927185.07924200001</v>
       </c>
+      <c r="ET24" s="13">
+        <v>934827.83995930001</v>
+      </c>
+      <c r="EU24" s="13">
+        <v>937725.01134129998</v>
+      </c>
+      <c r="EV24" s="13">
+        <v>939788.36928300001</v>
+      </c>
     </row>
-    <row r="25" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>14</v>
       </c>
@@ -11164,8 +11347,17 @@
       <c r="ES25" s="13">
         <v>319497.80196479999</v>
       </c>
+      <c r="ET25" s="13">
+        <v>340087.14952409995</v>
+      </c>
+      <c r="EU25" s="13">
+        <v>335487.16222170001</v>
+      </c>
+      <c r="EV25" s="13">
+        <v>309120.02989940002</v>
+      </c>
     </row>
-    <row r="26" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
@@ -11613,8 +11805,17 @@
       <c r="ES26" s="13">
         <v>455771.14479720005</v>
       </c>
+      <c r="ET26" s="13">
+        <v>454275.02361740003</v>
+      </c>
+      <c r="EU26" s="13">
+        <v>455106.28743909998</v>
+      </c>
+      <c r="EV26" s="13">
+        <v>460199.98545689997</v>
+      </c>
     </row>
-    <row r="27" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>6</v>
       </c>
@@ -12062,8 +12263,17 @@
       <c r="ES27" s="13">
         <v>21423.762398800172</v>
       </c>
+      <c r="ET27" s="13">
+        <v>20644.421730100061</v>
+      </c>
+      <c r="EU27" s="13">
+        <v>22102.864360699954</v>
+      </c>
+      <c r="EV27" s="13">
+        <v>24230.910966299882</v>
+      </c>
     </row>
-    <row r="28" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>7</v>
       </c>
@@ -12511,8 +12721,17 @@
       <c r="ES28" s="13">
         <v>17113.687977899997</v>
       </c>
+      <c r="ET28" s="13">
+        <v>16342.565352</v>
+      </c>
+      <c r="EU28" s="13">
+        <v>16412.9283325</v>
+      </c>
+      <c r="EV28" s="13">
+        <v>16517.755774899997</v>
+      </c>
     </row>
-    <row r="29" spans="1:149" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:152" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -12960,8 +13179,17 @@
       <c r="ES29" s="13">
         <v>4310.0744208999995</v>
       </c>
+      <c r="ET29" s="13">
+        <v>4301.8563781000003</v>
+      </c>
+      <c r="EU29" s="13">
+        <v>5689.9360281999998</v>
+      </c>
+      <c r="EV29" s="13">
+        <v>7713.1551914000001</v>
+      </c>
     </row>
-    <row r="30" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
@@ -13111,8 +13339,11 @@
       <c r="EQ30" s="14"/>
       <c r="ER30" s="14"/>
       <c r="ES30" s="14"/>
+      <c r="ET30" s="14"/>
+      <c r="EU30" s="14"/>
+      <c r="EV30" s="14"/>
     </row>
-    <row r="31" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>15</v>
       </c>
@@ -13264,8 +13495,11 @@
       <c r="EQ31" s="15"/>
       <c r="ER31" s="15"/>
       <c r="ES31" s="15"/>
+      <c r="ET31" s="15"/>
+      <c r="EU31" s="15"/>
+      <c r="EV31" s="15"/>
     </row>
-    <row r="32" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
@@ -13415,8 +13649,11 @@
       <c r="EQ32" s="16"/>
       <c r="ER32" s="16"/>
       <c r="ES32" s="16"/>
+      <c r="ET32" s="16"/>
+      <c r="EU32" s="16"/>
+      <c r="EV32" s="16"/>
     </row>
-    <row r="33" spans="1:149" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:152" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>19</v>
       </c>
@@ -13958,7 +14195,7 @@
         <v>5934.8376982904738</v>
       </c>
       <c r="EG33" s="14">
-        <f t="shared" ref="EG33:ES37" si="9">EG7-EF7</f>
+        <f t="shared" ref="EG33:EV37" si="9">EG7-EF7</f>
         <v>2052.3417412724812</v>
       </c>
       <c r="EH33" s="14">
@@ -14009,8 +14246,20 @@
         <f t="shared" si="9"/>
         <v>9681.7231667730957</v>
       </c>
+      <c r="ET33" s="14">
+        <f t="shared" si="9"/>
+        <v>9897.1361731746001</v>
+      </c>
+      <c r="EU33" s="14">
+        <f t="shared" si="9"/>
+        <v>2353.3059616272803</v>
+      </c>
+      <c r="EV33" s="14">
+        <f t="shared" si="9"/>
+        <v>21043.695994345122</v>
+      </c>
     </row>
-    <row r="34" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>22</v>
       </c>
@@ -14603,8 +14852,20 @@
         <f t="shared" si="9"/>
         <v>15484.110004227143</v>
       </c>
+      <c r="ET34" s="14">
+        <f t="shared" si="9"/>
+        <v>16059.510254925233</v>
+      </c>
+      <c r="EU34" s="14">
+        <f t="shared" si="9"/>
+        <v>-1766.4154297274072</v>
+      </c>
+      <c r="EV34" s="14">
+        <f t="shared" si="9"/>
+        <v>-38125.725751545164</v>
+      </c>
     </row>
-    <row r="35" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>2</v>
       </c>
@@ -15197,8 +15458,20 @@
         <f t="shared" si="9"/>
         <v>17055.717100899958</v>
       </c>
+      <c r="ET35" s="14">
+        <f t="shared" si="9"/>
+        <v>23788.086916700064</v>
+      </c>
+      <c r="EU35" s="14">
+        <f t="shared" si="9"/>
+        <v>-3146.7901936999406</v>
+      </c>
+      <c r="EV35" s="14">
+        <f t="shared" si="9"/>
+        <v>-527.49904410005547</v>
+      </c>
     </row>
-    <row r="36" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>3</v>
       </c>
@@ -15791,8 +16064,20 @@
         <f t="shared" si="9"/>
         <v>137.57079150003847</v>
       </c>
+      <c r="ET36" s="14">
+        <f t="shared" si="9"/>
+        <v>412.76436269993428</v>
+      </c>
+      <c r="EU36" s="14">
+        <f t="shared" si="9"/>
+        <v>479.92929040000308</v>
+      </c>
+      <c r="EV36" s="14">
+        <f t="shared" si="9"/>
+        <v>-38484.02927859989</v>
+      </c>
     </row>
-    <row r="37" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>17</v>
       </c>
@@ -16385,8 +16670,20 @@
         <f t="shared" si="9"/>
         <v>88.742884000006597</v>
       </c>
+      <c r="ET37" s="14">
+        <f t="shared" si="9"/>
+        <v>266.22865800000727</v>
+      </c>
+      <c r="EU37" s="14">
+        <f t="shared" si="9"/>
+        <v>88.742884999956004</v>
+      </c>
+      <c r="EV37" s="14">
+        <f t="shared" si="9"/>
+        <v>-35532.457310999976</v>
+      </c>
     </row>
-    <row r="38" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>23</v>
       </c>
@@ -16924,7 +17221,7 @@
         <v>330.27214399998775</v>
       </c>
       <c r="EF38" s="14">
-        <f t="shared" ref="EF38:ES42" si="13">EF12-EE12</f>
+        <f t="shared" ref="EF38:EV42" si="13">EF12-EE12</f>
         <v>110.09070699999575</v>
       </c>
       <c r="EG38" s="14">
@@ -16979,8 +17276,20 @@
         <f t="shared" si="13"/>
         <v>88.742884000006597</v>
       </c>
+      <c r="ET38" s="14">
+        <f t="shared" si="13"/>
+        <v>266.22865800000727</v>
+      </c>
+      <c r="EU38" s="14">
+        <f t="shared" si="13"/>
+        <v>88.742884999956004</v>
+      </c>
+      <c r="EV38" s="14">
+        <f t="shared" si="13"/>
+        <v>-35532.457310999976</v>
+      </c>
     </row>
-    <row r="39" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>24</v>
       </c>
@@ -17573,8 +17882,20 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
+      <c r="ET39" s="14">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="EU39" s="14">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="EV39" s="14">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="40" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>25</v>
       </c>
@@ -18167,8 +18488,20 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
+      <c r="ET40" s="14">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="EU40" s="14">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="EV40" s="14">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="41" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>26</v>
       </c>
@@ -18761,8 +19094,20 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
+      <c r="ET41" s="14">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="EU41" s="14">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="EV41" s="14">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="42" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>9</v>
       </c>
@@ -19355,8 +19700,20 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
+      <c r="ET42" s="14">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="EU42" s="14">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="EV42" s="14">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="43" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>10</v>
       </c>
@@ -19790,7 +20147,7 @@
         <v>0</v>
       </c>
       <c r="DF43" s="14">
-        <f t="shared" ref="DF43:ES47" si="16">-(DF17-DE17)</f>
+        <f t="shared" ref="DF43:EV47" si="16">-(DF17-DE17)</f>
         <v>17003.135245900001</v>
       </c>
       <c r="DG43" s="14">
@@ -19949,8 +20306,20 @@
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
+      <c r="ET43" s="14">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="EU43" s="14">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="EV43" s="14">
+        <f t="shared" si="16"/>
+        <v>3000.5122951000003</v>
+      </c>
     </row>
-    <row r="44" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>12</v>
       </c>
@@ -20543,8 +20912,20 @@
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
+      <c r="ET44" s="14">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="EU44" s="14">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="EV44" s="14">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="45" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>18</v>
       </c>
@@ -21137,8 +21518,20 @@
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
+      <c r="ET45" s="14">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="EU45" s="14">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="EV45" s="14">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="46" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>11</v>
       </c>
@@ -21731,8 +22124,20 @@
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
+      <c r="ET46" s="14">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="EU46" s="14">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="EV46" s="14">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="47" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>16</v>
       </c>
@@ -22325,8 +22730,20 @@
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
+      <c r="ET47" s="14">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="EU47" s="14">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="EV47" s="14">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>21</v>
       </c>
@@ -22620,7 +23037,7 @@
         <v>-3678.5371843058383</v>
       </c>
       <c r="BW48" s="14">
-        <f t="shared" ref="BW48:ES53" si="22">BW22-BV22</f>
+        <f t="shared" ref="BW48:EV53" si="22">BW22-BV22</f>
         <v>-4079.5047014922602</v>
       </c>
       <c r="BX48" s="14">
@@ -22919,8 +23336,20 @@
         <f t="shared" si="22"/>
         <v>-1709.1778881727951</v>
       </c>
+      <c r="ET48" s="14">
+        <f t="shared" si="22"/>
+        <v>-8141.3410244745901</v>
+      </c>
+      <c r="EU48" s="14">
+        <f t="shared" si="22"/>
+        <v>900.4454735723557</v>
+      </c>
+      <c r="EV48" s="14">
+        <f t="shared" si="22"/>
+        <v>885.80257115489803</v>
+      </c>
     </row>
-    <row r="49" spans="1:149" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:152" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="20" t="s">
         <v>4</v>
       </c>
@@ -23513,8 +23942,20 @@
         <f t="shared" si="22"/>
         <v>25165.833171000239</v>
       </c>
+      <c r="ET49" s="23">
+        <f t="shared" si="22"/>
+        <v>25956.646428099833</v>
+      </c>
+      <c r="EU49" s="23">
+        <f t="shared" si="22"/>
+        <v>586.89053189987317</v>
+      </c>
+      <c r="EV49" s="23">
+        <f t="shared" si="22"/>
+        <v>-17082.029757200042</v>
+      </c>
     </row>
-    <row r="50" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>5</v>
       </c>
@@ -24107,8 +24548,20 @@
         <f t="shared" si="22"/>
         <v>9568.1901369999396</v>
       </c>
+      <c r="ET50" s="14">
+        <f t="shared" si="22"/>
+        <v>7642.7607172999997</v>
+      </c>
+      <c r="EU50" s="14">
+        <f t="shared" si="22"/>
+        <v>2897.1713819999713</v>
+      </c>
+      <c r="EV50" s="14">
+        <f t="shared" si="22"/>
+        <v>2063.3579417000292</v>
+      </c>
     </row>
-    <row r="51" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>14</v>
       </c>
@@ -24701,8 +25154,20 @@
         <f t="shared" si="22"/>
         <v>18251.248129099957</v>
       </c>
+      <c r="ET51" s="14">
+        <f t="shared" si="22"/>
+        <v>20589.34755929996</v>
+      </c>
+      <c r="EU51" s="14">
+        <f t="shared" si="22"/>
+        <v>-4599.9873023999389</v>
+      </c>
+      <c r="EV51" s="14">
+        <f t="shared" si="22"/>
+        <v>-26367.132322299993</v>
+      </c>
     </row>
-    <row r="52" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>13</v>
       </c>
@@ -25295,8 +25760,20 @@
         <f t="shared" si="22"/>
         <v>-393.5551932999515</v>
       </c>
+      <c r="ET52" s="14">
+        <f t="shared" si="22"/>
+        <v>-1496.1211798000149</v>
+      </c>
+      <c r="EU52" s="14">
+        <f t="shared" si="22"/>
+        <v>831.26382169994758</v>
+      </c>
+      <c r="EV52" s="14">
+        <f t="shared" si="22"/>
+        <v>5093.698017799994</v>
+      </c>
     </row>
-    <row r="53" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>6</v>
       </c>
@@ -25889,8 +26366,20 @@
         <f t="shared" si="22"/>
         <v>-2260.0499017997063</v>
       </c>
+      <c r="ET53" s="14">
+        <f t="shared" si="22"/>
+        <v>-779.34066870011156</v>
+      </c>
+      <c r="EU53" s="14">
+        <f t="shared" si="22"/>
+        <v>1458.4426305998932</v>
+      </c>
+      <c r="EV53" s="14">
+        <f t="shared" si="22"/>
+        <v>2128.0466055999277</v>
+      </c>
     </row>
-    <row r="54" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>7</v>
       </c>
@@ -26444,7 +26933,7 @@
         <v>1598.3836406000009</v>
       </c>
       <c r="EJ54" s="14">
-        <f t="shared" ref="EJ54:ES54" si="28">EJ28-EI28</f>
+        <f t="shared" ref="EJ54:EV54" si="28">EJ28-EI28</f>
         <v>874.59308369999781</v>
       </c>
       <c r="EK54" s="14">
@@ -26483,8 +26972,20 @@
         <f t="shared" si="28"/>
         <v>-1833.7092870000015</v>
       </c>
+      <c r="ET54" s="14">
+        <f t="shared" si="28"/>
+        <v>-771.12262589999773</v>
+      </c>
+      <c r="EU54" s="14">
+        <f t="shared" si="28"/>
+        <v>70.362980500000049</v>
+      </c>
+      <c r="EV54" s="14">
+        <f t="shared" si="28"/>
+        <v>104.82744239999738</v>
+      </c>
     </row>
-    <row r="55" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>8</v>
       </c>
@@ -26618,7 +27119,7 @@
         <v>-36.071311499999865</v>
       </c>
       <c r="AI55" s="14">
-        <f t="shared" ref="AI55:ES55" si="29">AI29-AH29</f>
+        <f t="shared" ref="AI55:EV55" si="29">AI29-AH29</f>
         <v>-325.20539640000015</v>
       </c>
       <c r="AJ55" s="14">
@@ -27077,21 +27578,33 @@
         <f t="shared" si="29"/>
         <v>-426.34061480000037</v>
       </c>
+      <c r="ET55" s="14">
+        <f t="shared" si="29"/>
+        <v>-8.2180427999992389</v>
+      </c>
+      <c r="EU55" s="14">
+        <f t="shared" si="29"/>
+        <v>1388.0796500999995</v>
+      </c>
+      <c r="EV55" s="14">
+        <f t="shared" si="29"/>
+        <v>2023.2191632000004</v>
+      </c>
     </row>
-    <row r="56" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A56" s="4"/>
     </row>
-    <row r="57" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:152" x14ac:dyDescent="0.3">
       <c r="A57" s="17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="58" spans="1:149" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:152" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="59" spans="1:149" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:152" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A59" s="17" t="s">
         <v>31</v>
       </c>
@@ -27232,13 +27745,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BED68AD-6C03-4B9E-9EA8-146A56A90F60}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E3B7E8C-7B66-4819-ADF4-F6812664EF2C}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD7E6576-F2A8-4E84-91AB-AB1C679112A6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1023B2A1-D799-43FB-BED5-E0395D7FE4AF}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B00E855-B3BF-4229-B57F-FD5D407B0911}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A8E47A1-933A-41BB-B574-219FC145BF11}"/>
 </file>
</xml_diff>

<commit_message>
Auto commit - 2024-09-20
</commit_message>
<xml_diff>
--- a/2024/2024_06_07_CB_loans/2_Money_Base_dayly_eng.xlsx
+++ b/2024/2024_06_07_CB_loans/2_Money_Base_dayly_eng.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D50FA5-ADE2-40E4-9803-FB5C12110014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA84993-05E7-4C90-8371-CC41BC9E59BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="205">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -708,6 +708,18 @@
   </si>
   <si>
     <t>11.09.24</t>
+  </si>
+  <si>
+    <t>12.09.24</t>
+  </si>
+  <si>
+    <t>13.09.24</t>
+  </si>
+  <si>
+    <t>16.09.24</t>
+  </si>
+  <si>
+    <t>17.09.24</t>
   </si>
 </sst>
 </file>
@@ -2069,13 +2081,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:FU59"/>
+  <dimension ref="A1:FY59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="DU7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="FX24" sqref="FX24"/>
+      <selection pane="bottomRight" activeCell="GD27" sqref="GD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2097,27 +2109,27 @@
     <col min="126" max="146" width="16" style="7" hidden="1" customWidth="1"/>
     <col min="147" max="147" width="16" style="7" bestFit="1" customWidth="1"/>
     <col min="148" max="168" width="16" style="7" hidden="1" customWidth="1"/>
-    <col min="169" max="177" width="16" style="7" bestFit="1" customWidth="1"/>
-    <col min="178" max="16384" width="11.5703125" style="7"/>
+    <col min="169" max="181" width="16" style="7" bestFit="1" customWidth="1"/>
+    <col min="182" max="16384" width="11.5703125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:177" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:181" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:177" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:181" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:177" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:181" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
     </row>
-    <row r="4" spans="1:177" ht="3" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:181" ht="3" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
     </row>
-    <row r="5" spans="1:177" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:181" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -2649,8 +2661,20 @@
       <c r="FU5" s="10" t="s">
         <v>200</v>
       </c>
+      <c r="FV5" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="FW5" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="FX5" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="FY5" s="10" t="s">
+        <v>204</v>
+      </c>
     </row>
-    <row r="6" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
@@ -2828,8 +2852,12 @@
       <c r="FS6" s="12"/>
       <c r="FT6" s="12"/>
       <c r="FU6" s="12"/>
+      <c r="FV6" s="12"/>
+      <c r="FW6" s="12"/>
+      <c r="FX6" s="12"/>
+      <c r="FY6" s="12"/>
     </row>
-    <row r="7" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
@@ -3361,8 +3389,20 @@
       <c r="FU7" s="13">
         <v>1035243.9947972189</v>
       </c>
+      <c r="FV7" s="13">
+        <v>1036736.6260914579</v>
+      </c>
+      <c r="FW7" s="13">
+        <v>1036583.2750369236</v>
+      </c>
+      <c r="FX7" s="13">
+        <v>1046252.4712205735</v>
+      </c>
+      <c r="FY7" s="13">
+        <v>1052006.7072076763</v>
+      </c>
     </row>
-    <row r="8" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
@@ -3894,8 +3934,20 @@
       <c r="FU8" s="13">
         <v>731363.38459338096</v>
       </c>
+      <c r="FV8" s="13">
+        <v>733994.98564524227</v>
+      </c>
+      <c r="FW8" s="13">
+        <v>735431.21183657646</v>
+      </c>
+      <c r="FX8" s="13">
+        <v>738756.71303922671</v>
+      </c>
+      <c r="FY8" s="13">
+        <v>723313.64539292385</v>
+      </c>
     </row>
-    <row r="9" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -4427,8 +4479,20 @@
       <c r="FU9" s="13">
         <v>-426145.16768129996</v>
       </c>
+      <c r="FV9" s="13">
+        <v>-424046.85327730002</v>
+      </c>
+      <c r="FW9" s="13">
+        <v>-421873.51202609995</v>
+      </c>
+      <c r="FX9" s="13">
+        <v>-412670.88951030013</v>
+      </c>
+      <c r="FY9" s="13">
+        <v>-427941.28486020002</v>
+      </c>
     </row>
-    <row r="10" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
@@ -4960,8 +5024,20 @@
       <c r="FU10" s="13">
         <v>711558.63176159991</v>
       </c>
+      <c r="FV10" s="13">
+        <v>711692.29375169997</v>
+      </c>
+      <c r="FW10" s="13">
+        <v>711882.09314580006</v>
+      </c>
+      <c r="FX10" s="13">
+        <v>712283.18571799994</v>
+      </c>
+      <c r="FY10" s="13">
+        <v>712552.54946680006</v>
+      </c>
     </row>
-    <row r="11" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -5493,8 +5569,20 @@
       <c r="FU11" s="13">
         <v>398000</v>
       </c>
+      <c r="FV11" s="13">
+        <v>398082.910691</v>
+      </c>
+      <c r="FW11" s="13">
+        <v>398165.82137800002</v>
+      </c>
+      <c r="FX11" s="13">
+        <v>398414.55344499997</v>
+      </c>
+      <c r="FY11" s="13">
+        <v>398497.464133</v>
+      </c>
     </row>
-    <row r="12" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
@@ -6026,8 +6114,20 @@
       <c r="FU12" s="13">
         <v>398000</v>
       </c>
+      <c r="FV12" s="13">
+        <v>398082.910691</v>
+      </c>
+      <c r="FW12" s="13">
+        <v>398165.82137800002</v>
+      </c>
+      <c r="FX12" s="13">
+        <v>398414.55344500003</v>
+      </c>
+      <c r="FY12" s="13">
+        <v>398497.464133</v>
+      </c>
     </row>
-    <row r="13" spans="1:177" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:181" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -6559,8 +6659,20 @@
       <c r="FU13" s="13">
         <v>0</v>
       </c>
+      <c r="FV13" s="13">
+        <v>0</v>
+      </c>
+      <c r="FW13" s="13">
+        <v>0</v>
+      </c>
+      <c r="FX13" s="13">
+        <v>0</v>
+      </c>
+      <c r="FY13" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
@@ -7092,8 +7204,20 @@
       <c r="FU14" s="13">
         <v>0</v>
       </c>
+      <c r="FV14" s="13">
+        <v>0</v>
+      </c>
+      <c r="FW14" s="13">
+        <v>0</v>
+      </c>
+      <c r="FX14" s="13">
+        <v>0</v>
+      </c>
+      <c r="FY14" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
@@ -7625,8 +7749,20 @@
       <c r="FU15" s="13">
         <v>0</v>
       </c>
+      <c r="FV15" s="13">
+        <v>0</v>
+      </c>
+      <c r="FW15" s="13">
+        <v>0</v>
+      </c>
+      <c r="FX15" s="13">
+        <v>0</v>
+      </c>
+      <c r="FY15" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
@@ -8158,8 +8294,20 @@
       <c r="FU16" s="13">
         <v>0</v>
       </c>
+      <c r="FV16" s="13">
+        <v>0</v>
+      </c>
+      <c r="FW16" s="13">
+        <v>0</v>
+      </c>
+      <c r="FX16" s="13">
+        <v>0</v>
+      </c>
+      <c r="FY16" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
@@ -8691,8 +8839,20 @@
       <c r="FU17" s="13">
         <v>0</v>
       </c>
+      <c r="FV17" s="13">
+        <v>0</v>
+      </c>
+      <c r="FW17" s="13">
+        <v>0</v>
+      </c>
+      <c r="FX17" s="13">
+        <v>0</v>
+      </c>
+      <c r="FY17" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
@@ -9224,8 +9384,20 @@
       <c r="FU18" s="13">
         <v>0</v>
       </c>
+      <c r="FV18" s="13">
+        <v>0</v>
+      </c>
+      <c r="FW18" s="13">
+        <v>0</v>
+      </c>
+      <c r="FX18" s="13">
+        <v>0</v>
+      </c>
+      <c r="FY18" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
@@ -9757,8 +9929,20 @@
       <c r="FU19" s="13">
         <v>0</v>
       </c>
+      <c r="FV19" s="13">
+        <v>0</v>
+      </c>
+      <c r="FW19" s="13">
+        <v>0</v>
+      </c>
+      <c r="FX19" s="13">
+        <v>0</v>
+      </c>
+      <c r="FY19" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:177" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:181" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>11</v>
       </c>
@@ -10290,8 +10474,20 @@
       <c r="FU20" s="13">
         <v>0</v>
       </c>
+      <c r="FV20" s="13">
+        <v>0</v>
+      </c>
+      <c r="FW20" s="13">
+        <v>0</v>
+      </c>
+      <c r="FX20" s="13">
+        <v>0</v>
+      </c>
+      <c r="FY20" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
@@ -10823,8 +11019,20 @@
       <c r="FU21" s="13">
         <v>0</v>
       </c>
+      <c r="FV21" s="13">
+        <v>0</v>
+      </c>
+      <c r="FW21" s="13">
+        <v>0</v>
+      </c>
+      <c r="FX21" s="13">
+        <v>0</v>
+      </c>
+      <c r="FY21" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -11356,8 +11564,20 @@
       <c r="FU22" s="13">
         <v>445949.92051308102</v>
       </c>
+      <c r="FV22" s="13">
+        <v>446349.54517084232</v>
+      </c>
+      <c r="FW22" s="13">
+        <v>445422.63071687636</v>
+      </c>
+      <c r="FX22" s="13">
+        <v>439144.41683152691</v>
+      </c>
+      <c r="FY22" s="13">
+        <v>438702.3807863238</v>
+      </c>
     </row>
-    <row r="23" spans="1:177" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:181" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
         <v>4</v>
       </c>
@@ -11889,8 +12109,20 @@
       <c r="FU23" s="21">
         <v>1766607.3793905999</v>
       </c>
+      <c r="FV23" s="21">
+        <v>1770731.6117367002</v>
+      </c>
+      <c r="FW23" s="21">
+        <v>1772014.4868735</v>
+      </c>
+      <c r="FX23" s="21">
+        <v>1785009.1842598002</v>
+      </c>
+      <c r="FY23" s="21">
+        <v>1775320.3526006001</v>
+      </c>
     </row>
-    <row r="24" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>5</v>
       </c>
@@ -12422,8 +12654,20 @@
       <c r="FU24" s="13">
         <v>947734.13839219999</v>
       </c>
+      <c r="FV24" s="13">
+        <v>945022.13815889996</v>
+      </c>
+      <c r="FW24" s="13">
+        <v>946409.60510220006</v>
+      </c>
+      <c r="FX24" s="13">
+        <v>947812.13732840004</v>
+      </c>
+      <c r="FY24" s="13">
+        <v>944195.77111839992</v>
+      </c>
     </row>
-    <row r="25" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>14</v>
       </c>
@@ -12955,8 +13199,20 @@
       <c r="FU25" s="13">
         <v>352512.63923940004</v>
       </c>
+      <c r="FV25" s="13">
+        <v>356856.39227779995</v>
+      </c>
+      <c r="FW25" s="13">
+        <v>356123.40039979998</v>
+      </c>
+      <c r="FX25" s="13">
+        <v>368612.61884220003</v>
+      </c>
+      <c r="FY25" s="13">
+        <v>355446.14335870004</v>
+      </c>
     </row>
-    <row r="26" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
@@ -13488,8 +13744,20 @@
       <c r="FU26" s="13">
         <v>446496.36594280001</v>
       </c>
+      <c r="FV26" s="13">
+        <v>449827.62144300004</v>
+      </c>
+      <c r="FW26" s="13">
+        <v>450528.44042</v>
+      </c>
+      <c r="FX26" s="13">
+        <v>449175.89323290001</v>
+      </c>
+      <c r="FY26" s="13">
+        <v>455386.19406890008</v>
+      </c>
     </row>
-    <row r="27" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>6</v>
       </c>
@@ -14021,8 +14289,20 @@
       <c r="FU27" s="13">
         <v>19864.235816199856</v>
       </c>
+      <c r="FV27" s="13">
+        <v>19025.459857000213</v>
+      </c>
+      <c r="FW27" s="13">
+        <v>18953.040951500006</v>
+      </c>
+      <c r="FX27" s="13">
+        <v>19408.534856300161</v>
+      </c>
+      <c r="FY27" s="13">
+        <v>20292.244054600073</v>
+      </c>
     </row>
-    <row r="28" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>7</v>
       </c>
@@ -14554,8 +14834,20 @@
       <c r="FU28" s="13">
         <v>15972.224909400002</v>
       </c>
+      <c r="FV28" s="13">
+        <v>15811.390681199999</v>
+      </c>
+      <c r="FW28" s="13">
+        <v>15726.910669299999</v>
+      </c>
+      <c r="FX28" s="13">
+        <v>16203.631069200001</v>
+      </c>
+      <c r="FY28" s="13">
+        <v>16375.451503800001</v>
+      </c>
     </row>
-    <row r="29" spans="1:177" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:181" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -15087,8 +15379,20 @@
       <c r="FU29" s="13">
         <v>3892.0109068000002</v>
       </c>
+      <c r="FV29" s="13">
+        <v>3214.0691758000003</v>
+      </c>
+      <c r="FW29" s="13">
+        <v>3226.1302821999998</v>
+      </c>
+      <c r="FX29" s="13">
+        <v>3204.9037871</v>
+      </c>
+      <c r="FY29" s="13">
+        <v>3916.7925508000003</v>
+      </c>
     </row>
-    <row r="30" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
@@ -15266,8 +15570,12 @@
       <c r="FS30" s="14"/>
       <c r="FT30" s="14"/>
       <c r="FU30" s="14"/>
+      <c r="FV30" s="14"/>
+      <c r="FW30" s="14"/>
+      <c r="FX30" s="14"/>
+      <c r="FY30" s="14"/>
     </row>
-    <row r="31" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>15</v>
       </c>
@@ -15447,8 +15755,12 @@
       <c r="FS31" s="15"/>
       <c r="FT31" s="15"/>
       <c r="FU31" s="15"/>
+      <c r="FV31" s="15"/>
+      <c r="FW31" s="15"/>
+      <c r="FX31" s="15"/>
+      <c r="FY31" s="15"/>
     </row>
-    <row r="32" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
@@ -15626,8 +15938,12 @@
       <c r="FS32" s="16"/>
       <c r="FT32" s="16"/>
       <c r="FU32" s="16"/>
+      <c r="FV32" s="16"/>
+      <c r="FW32" s="16"/>
+      <c r="FX32" s="16"/>
+      <c r="FY32" s="16"/>
     </row>
-    <row r="33" spans="1:177" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:181" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>19</v>
       </c>
@@ -16241,7 +16557,7 @@
         <v>521.48554795375094</v>
       </c>
       <c r="EY33" s="14">
-        <f t="shared" ref="EY33:FU42" si="13">EY7-EX7</f>
+        <f t="shared" ref="EY33:FY42" si="13">EY7-EX7</f>
         <v>1842.3852793342667</v>
       </c>
       <c r="EZ33" s="14">
@@ -16281,7 +16597,7 @@
         <v>19966.335642270511</v>
       </c>
       <c r="FI33" s="14">
-        <f t="shared" ref="FI33:FU33" si="15">FI7-FH7</f>
+        <f t="shared" ref="FI33:FY33" si="15">FI7-FH7</f>
         <v>-5674.7591277488973</v>
       </c>
       <c r="FJ33" s="14">
@@ -16332,8 +16648,24 @@
         <f t="shared" si="15"/>
         <v>-5959.5796642255737</v>
       </c>
+      <c r="FV33" s="14">
+        <f t="shared" si="15"/>
+        <v>1492.6312942389632</v>
+      </c>
+      <c r="FW33" s="14">
+        <f t="shared" si="15"/>
+        <v>-153.35105453431606</v>
+      </c>
+      <c r="FX33" s="14">
+        <f t="shared" si="15"/>
+        <v>9669.1961836499395</v>
+      </c>
+      <c r="FY33" s="14">
+        <f t="shared" si="15"/>
+        <v>5754.2359871027293</v>
+      </c>
     </row>
-    <row r="34" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>22</v>
       </c>
@@ -17038,8 +17370,24 @@
         <f t="shared" si="13"/>
         <v>71868.367817625753</v>
       </c>
+      <c r="FV34" s="14">
+        <f t="shared" si="13"/>
+        <v>2631.6010518613039</v>
+      </c>
+      <c r="FW34" s="14">
+        <f t="shared" si="13"/>
+        <v>1436.2261913341936</v>
+      </c>
+      <c r="FX34" s="14">
+        <f t="shared" si="13"/>
+        <v>3325.5012026502518</v>
+      </c>
+      <c r="FY34" s="14">
+        <f t="shared" si="13"/>
+        <v>-15443.067646302865</v>
+      </c>
     </row>
-    <row r="35" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>2</v>
       </c>
@@ -17744,8 +18092,24 @@
         <f t="shared" si="13"/>
         <v>-23668.768599099887</v>
       </c>
+      <c r="FV35" s="14">
+        <f t="shared" si="13"/>
+        <v>2098.3144039999461</v>
+      </c>
+      <c r="FW35" s="14">
+        <f t="shared" si="13"/>
+        <v>2173.341251200065</v>
+      </c>
+      <c r="FX35" s="14">
+        <f t="shared" si="13"/>
+        <v>9202.6225157998269</v>
+      </c>
+      <c r="FY35" s="14">
+        <f t="shared" si="13"/>
+        <v>-15270.395349899889</v>
+      </c>
     </row>
-    <row r="36" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>3</v>
       </c>
@@ -18450,8 +18814,24 @@
         <f t="shared" si="13"/>
         <v>96385.7739899999</v>
       </c>
+      <c r="FV36" s="14">
+        <f t="shared" si="13"/>
+        <v>133.66199010005221</v>
+      </c>
+      <c r="FW36" s="14">
+        <f t="shared" si="13"/>
+        <v>189.79939410008956</v>
+      </c>
+      <c r="FX36" s="14">
+        <f t="shared" si="13"/>
+        <v>401.09257219987921</v>
+      </c>
+      <c r="FY36" s="14">
+        <f t="shared" si="13"/>
+        <v>269.3637488001259</v>
+      </c>
     </row>
-    <row r="37" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>17</v>
       </c>
@@ -19156,8 +19536,24 @@
         <f t="shared" si="13"/>
         <v>29323.590490999981</v>
       </c>
+      <c r="FV37" s="14">
+        <f t="shared" si="13"/>
+        <v>82.910690999997314</v>
+      </c>
+      <c r="FW37" s="14">
+        <f t="shared" si="13"/>
+        <v>82.910687000025064</v>
+      </c>
+      <c r="FX37" s="14">
+        <f t="shared" si="13"/>
+        <v>248.73206699994626</v>
+      </c>
+      <c r="FY37" s="14">
+        <f t="shared" si="13"/>
+        <v>82.910688000032678</v>
+      </c>
     </row>
-    <row r="38" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>23</v>
       </c>
@@ -19862,8 +20258,24 @@
         <f t="shared" si="13"/>
         <v>29323.590490999981</v>
       </c>
+      <c r="FV38" s="14">
+        <f t="shared" si="13"/>
+        <v>82.910690999997314</v>
+      </c>
+      <c r="FW38" s="14">
+        <f t="shared" si="13"/>
+        <v>82.910687000025064</v>
+      </c>
+      <c r="FX38" s="14">
+        <f t="shared" si="13"/>
+        <v>248.73206700000446</v>
+      </c>
+      <c r="FY38" s="14">
+        <f t="shared" si="13"/>
+        <v>82.910687999974471</v>
+      </c>
     </row>
-    <row r="39" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>24</v>
       </c>
@@ -20568,8 +20980,24 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
+      <c r="FV39" s="14">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="FW39" s="14">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="FX39" s="14">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="FY39" s="14">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="40" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>25</v>
       </c>
@@ -21274,8 +21702,24 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
+      <c r="FV40" s="14">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="FW40" s="14">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="FX40" s="14">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="FY40" s="14">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="41" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>26</v>
       </c>
@@ -21980,8 +22424,24 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
+      <c r="FV41" s="14">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="FW41" s="14">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="FX41" s="14">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="FY41" s="14">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="42" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>9</v>
       </c>
@@ -22686,8 +23146,24 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
+      <c r="FV42" s="14">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="FW42" s="14">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="FX42" s="14">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="FY42" s="14">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="43" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>10</v>
       </c>
@@ -23301,7 +23777,7 @@
         <v>18003.073770499999</v>
       </c>
       <c r="EY43" s="14">
-        <f t="shared" ref="EY43:FU47" si="25">-(EY17-EX17)</f>
+        <f t="shared" ref="EY43:FY47" si="25">-(EY17-EX17)</f>
         <v>46407.923497399999</v>
       </c>
       <c r="EZ43" s="14">
@@ -23392,8 +23868,24 @@
         <f t="shared" si="25"/>
         <v>-67011.441256999999</v>
       </c>
+      <c r="FV43" s="14">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="FW43" s="14">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="FX43" s="14">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="FY43" s="14">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="44" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>12</v>
       </c>
@@ -24098,8 +24590,24 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
+      <c r="FV44" s="14">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="FW44" s="14">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="FX44" s="14">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="FY44" s="14">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="45" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>18</v>
       </c>
@@ -24804,8 +25312,24 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
+      <c r="FV45" s="14">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="FW45" s="14">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="FX45" s="14">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="FY45" s="14">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="46" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>11</v>
       </c>
@@ -25510,8 +26034,24 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
+      <c r="FV46" s="14">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="FW46" s="14">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="FX46" s="14">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="FY46" s="14">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="47" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>16</v>
       </c>
@@ -26216,8 +26756,24 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
+      <c r="FV47" s="14">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="FW47" s="14">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="FX47" s="14">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="FY47" s="14">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>21</v>
       </c>
@@ -26831,7 +27387,7 @@
         <v>2505.4083482458955</v>
       </c>
       <c r="EY48" s="14">
-        <f t="shared" ref="EY48:FU55" si="38">EY22-EX22</f>
+        <f t="shared" ref="EY48:FY55" si="38">EY22-EX22</f>
         <v>-3873.0712501335656</v>
       </c>
       <c r="EZ48" s="14">
@@ -26922,8 +27478,24 @@
         <f t="shared" si="38"/>
         <v>-848.63757327431813</v>
       </c>
+      <c r="FV48" s="14">
+        <f t="shared" si="38"/>
+        <v>399.62465776130557</v>
+      </c>
+      <c r="FW48" s="14">
+        <f t="shared" si="38"/>
+        <v>-926.914453965961</v>
+      </c>
+      <c r="FX48" s="14">
+        <f t="shared" si="38"/>
+        <v>-6278.2138853494544</v>
+      </c>
+      <c r="FY48" s="14">
+        <f t="shared" si="38"/>
+        <v>-442.03604520310182</v>
+      </c>
     </row>
-    <row r="49" spans="1:177" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:181" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="20" t="s">
         <v>4</v>
       </c>
@@ -27628,8 +28200,24 @@
         <f t="shared" si="38"/>
         <v>65908.788153400179</v>
       </c>
+      <c r="FV49" s="23">
+        <f t="shared" si="38"/>
+        <v>4124.232346100267</v>
+      </c>
+      <c r="FW49" s="23">
+        <f t="shared" si="38"/>
+        <v>1282.8751367998775</v>
+      </c>
+      <c r="FX49" s="23">
+        <f t="shared" si="38"/>
+        <v>12994.697386300191</v>
+      </c>
+      <c r="FY49" s="23">
+        <f t="shared" si="38"/>
+        <v>-9688.8316592001356</v>
+      </c>
     </row>
-    <row r="50" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>5</v>
       </c>
@@ -28334,8 +28922,24 @@
         <f t="shared" si="38"/>
         <v>-4299.0375200000126</v>
       </c>
+      <c r="FV50" s="14">
+        <f t="shared" si="38"/>
+        <v>-2712.0002333000302</v>
+      </c>
+      <c r="FW50" s="14">
+        <f t="shared" si="38"/>
+        <v>1387.4669433000963</v>
+      </c>
+      <c r="FX50" s="14">
+        <f t="shared" si="38"/>
+        <v>1402.5322261999827</v>
+      </c>
+      <c r="FY50" s="14">
+        <f t="shared" si="38"/>
+        <v>-3616.3662100001238</v>
+      </c>
     </row>
-    <row r="51" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>14</v>
       </c>
@@ -29040,8 +29644,24 @@
         <f t="shared" si="38"/>
         <v>76479.484728300071</v>
       </c>
+      <c r="FV51" s="14">
+        <f t="shared" si="38"/>
+        <v>4343.753038399911</v>
+      </c>
+      <c r="FW51" s="14">
+        <f t="shared" si="38"/>
+        <v>-732.99187799997162</v>
+      </c>
+      <c r="FX51" s="14">
+        <f t="shared" si="38"/>
+        <v>12489.218442400044</v>
+      </c>
+      <c r="FY51" s="14">
+        <f t="shared" si="38"/>
+        <v>-13166.475483499991</v>
+      </c>
     </row>
-    <row r="52" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>13</v>
       </c>
@@ -29746,8 +30366,24 @@
         <f t="shared" si="38"/>
         <v>-6402.5661017999519</v>
       </c>
+      <c r="FV52" s="14">
+        <f t="shared" si="38"/>
+        <v>3331.2555002000299</v>
+      </c>
+      <c r="FW52" s="14">
+        <f t="shared" si="38"/>
+        <v>700.81897699995898</v>
+      </c>
+      <c r="FX52" s="14">
+        <f t="shared" si="38"/>
+        <v>-1352.54718709999</v>
+      </c>
+      <c r="FY52" s="14">
+        <f t="shared" si="38"/>
+        <v>6210.3008360000676</v>
+      </c>
     </row>
-    <row r="53" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>6</v>
       </c>
@@ -30452,8 +31088,24 @@
         <f t="shared" si="38"/>
         <v>130.9070469000726</v>
       </c>
+      <c r="FV53" s="14">
+        <f t="shared" si="38"/>
+        <v>-838.77595919964369</v>
+      </c>
+      <c r="FW53" s="14">
+        <f t="shared" si="38"/>
+        <v>-72.418905500206165</v>
+      </c>
+      <c r="FX53" s="14">
+        <f t="shared" si="38"/>
+        <v>455.49390480015427</v>
+      </c>
+      <c r="FY53" s="14">
+        <f t="shared" si="38"/>
+        <v>883.7091982999118</v>
+      </c>
     </row>
-    <row r="54" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>7</v>
       </c>
@@ -31158,8 +31810,24 @@
         <f t="shared" si="38"/>
         <v>170.64131980000275</v>
       </c>
+      <c r="FV54" s="14">
+        <f t="shared" si="38"/>
+        <v>-160.83422820000305</v>
+      </c>
+      <c r="FW54" s="14">
+        <f t="shared" si="38"/>
+        <v>-84.480011899999226</v>
+      </c>
+      <c r="FX54" s="14">
+        <f t="shared" si="38"/>
+        <v>476.72039990000121</v>
+      </c>
+      <c r="FY54" s="14">
+        <f t="shared" si="38"/>
+        <v>171.82043460000023</v>
+      </c>
     </row>
-    <row r="55" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>8</v>
       </c>
@@ -31864,21 +32532,37 @@
         <f t="shared" si="38"/>
         <v>-39.734272899999723</v>
       </c>
+      <c r="FV55" s="14">
+        <f t="shared" si="38"/>
+        <v>-677.94173099999989</v>
+      </c>
+      <c r="FW55" s="14">
+        <f t="shared" si="38"/>
+        <v>12.061106399999517</v>
+      </c>
+      <c r="FX55" s="14">
+        <f t="shared" si="38"/>
+        <v>-21.226495099999738</v>
+      </c>
+      <c r="FY55" s="14">
+        <f t="shared" si="38"/>
+        <v>711.88876370000025</v>
+      </c>
     </row>
-    <row r="56" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A56" s="4"/>
     </row>
-    <row r="57" spans="1:177" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:181" x14ac:dyDescent="0.3">
       <c r="A57" s="17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="58" spans="1:177" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:181" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="59" spans="1:177" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:181" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A59" s="17" t="s">
         <v>31</v>
       </c>
@@ -32019,13 +32703,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{558F9A73-AC77-49A6-B25C-3FE130AFDB7C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D04630B8-D9C7-489F-B6C2-D442906960AB}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FE9727E-23FA-4561-8F49-8BBCAEB10822}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4AB0F629-211B-4E5A-9F99-5BE726D3516D}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5484BD3-0472-485D-8C5D-3BC4425FAE30}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96287BA8-9E4D-4009-A1E6-F0297ACCBE1C}"/>
 </file>
</xml_diff>

<commit_message>
Auto commit - 2024-12-09
</commit_message>
<xml_diff>
--- a/2024/2024_06_07_CB_loans/2_Money_Base_dayly_eng.xlsx
+++ b/2024/2024_06_07_CB_loans/2_Money_Base_dayly_eng.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0648CF85-2FBC-4F05-B429-17B94441DBC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411F6861-BCC7-4E55-B561-953D3DFF5E6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name=" Eng actual exchange rate" sheetId="4" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="255">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -811,6 +811,21 @@
   </si>
   <si>
     <t>19.11.24</t>
+  </si>
+  <si>
+    <t>20.11.24</t>
+  </si>
+  <si>
+    <t>21.11.24</t>
+  </si>
+  <si>
+    <t>22.11.24</t>
+  </si>
+  <si>
+    <t>25.11.24</t>
+  </si>
+  <si>
+    <t>26.11.24</t>
   </si>
 </sst>
 </file>
@@ -2159,13 +2174,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:HR63"/>
+  <dimension ref="A1:HW63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="GH7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="HS7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="HH26" sqref="HH26"/>
+      <selection pane="bottomRight" activeCell="HW5" sqref="HW5:HW31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2191,27 +2206,27 @@
     <col min="170" max="189" width="16" style="7" hidden="1" customWidth="1"/>
     <col min="190" max="190" width="16" style="7" bestFit="1" customWidth="1"/>
     <col min="191" max="212" width="16" style="7" hidden="1" customWidth="1"/>
-    <col min="213" max="226" width="16" style="7" bestFit="1" customWidth="1"/>
-    <col min="227" max="16384" width="11.5703125" style="7"/>
+    <col min="213" max="231" width="16" style="7" bestFit="1" customWidth="1"/>
+    <col min="232" max="16384" width="11.5703125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:226" s="24" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:231" s="24" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:226" s="24" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:231" s="24" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:226" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:231" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
     </row>
-    <row r="4" spans="1:226" ht="3" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:231" ht="3" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
     </row>
-    <row r="5" spans="1:226" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:231" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -2890,8 +2905,23 @@
       <c r="HR5" s="10" t="s">
         <v>249</v>
       </c>
+      <c r="HS5" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="HT5" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="HU5" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="HV5" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="HW5" s="10" t="s">
+        <v>254</v>
+      </c>
     </row>
-    <row r="6" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
@@ -3118,8 +3148,13 @@
       <c r="HP6" s="12"/>
       <c r="HQ6" s="12"/>
       <c r="HR6" s="12"/>
+      <c r="HS6" s="12"/>
+      <c r="HT6" s="12"/>
+      <c r="HU6" s="12"/>
+      <c r="HV6" s="12"/>
+      <c r="HW6" s="12"/>
     </row>
-    <row r="7" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -3798,8 +3833,23 @@
       <c r="HR7" s="13">
         <v>1016585.8898607745</v>
       </c>
+      <c r="HS7" s="13">
+        <v>1008414.4287661719</v>
+      </c>
+      <c r="HT7" s="13">
+        <v>1010645.2770444253</v>
+      </c>
+      <c r="HU7" s="13">
+        <v>1017219.4444601584</v>
+      </c>
+      <c r="HV7" s="13">
+        <v>1028605.8998586724</v>
+      </c>
+      <c r="HW7" s="13">
+        <v>1064695.7498585761</v>
+      </c>
     </row>
-    <row r="8" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
@@ -4478,8 +4528,23 @@
       <c r="HR8" s="13">
         <v>678479.02597642539</v>
       </c>
+      <c r="HS8" s="13">
+        <v>781643.87991762813</v>
+      </c>
+      <c r="HT8" s="13">
+        <v>778620.29866317473</v>
+      </c>
+      <c r="HU8" s="13">
+        <v>769467.41031434189</v>
+      </c>
+      <c r="HV8" s="13">
+        <v>766547.32582822721</v>
+      </c>
+      <c r="HW8" s="13">
+        <v>734487.8255758239</v>
+      </c>
     </row>
-    <row r="9" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -5158,8 +5223,23 @@
       <c r="HR9" s="13">
         <v>-400884.40084740001</v>
       </c>
+      <c r="HS9" s="13">
+        <v>-419634.43399249995</v>
+      </c>
+      <c r="HT9" s="13">
+        <v>-422608.06374170003</v>
+      </c>
+      <c r="HU9" s="13">
+        <v>-432319.00514740002</v>
+      </c>
+      <c r="HV9" s="13">
+        <v>-430655.79538290005</v>
+      </c>
+      <c r="HW9" s="13">
+        <v>-467495.77825729997</v>
+      </c>
     </row>
-    <row r="10" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
@@ -5838,8 +5918,23 @@
       <c r="HR10" s="13">
         <v>644720.21630779991</v>
       </c>
+      <c r="HS10" s="13">
+        <v>765848.42129739991</v>
+      </c>
+      <c r="HT10" s="13">
+        <v>765856.61270130018</v>
+      </c>
+      <c r="HU10" s="13">
+        <v>766167.07289049996</v>
+      </c>
+      <c r="HV10" s="13">
+        <v>766594.99967079994</v>
+      </c>
+      <c r="HW10" s="13">
+        <v>773204.13847960008</v>
+      </c>
     </row>
-    <row r="11" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -6518,8 +6613,23 @@
       <c r="HR11" s="13">
         <v>345419.72565700003</v>
       </c>
+      <c r="HS11" s="13">
+        <v>466500</v>
+      </c>
+      <c r="HT11" s="13">
+        <v>466594.677922</v>
+      </c>
+      <c r="HU11" s="13">
+        <v>466689.35584199999</v>
+      </c>
+      <c r="HV11" s="13">
+        <v>466973.389601</v>
+      </c>
+      <c r="HW11" s="13">
+        <v>467068.06752600003</v>
+      </c>
     </row>
-    <row r="12" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -7198,8 +7308,23 @@
       <c r="HR12" s="13">
         <v>345419.72565699997</v>
       </c>
+      <c r="HS12" s="13">
+        <v>365000</v>
+      </c>
+      <c r="HT12" s="13">
+        <v>365074.25713099999</v>
+      </c>
+      <c r="HU12" s="13">
+        <v>365148.51426500001</v>
+      </c>
+      <c r="HV12" s="13">
+        <v>365371.28565500001</v>
+      </c>
+      <c r="HW12" s="13">
+        <v>365445.54278900003</v>
+      </c>
     </row>
-    <row r="13" spans="1:226" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:231" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
@@ -7878,8 +8003,23 @@
       <c r="HR13" s="13">
         <v>0</v>
       </c>
+      <c r="HS13" s="13">
+        <v>0</v>
+      </c>
+      <c r="HT13" s="13">
+        <v>0</v>
+      </c>
+      <c r="HU13" s="13">
+        <v>0</v>
+      </c>
+      <c r="HV13" s="13">
+        <v>0</v>
+      </c>
+      <c r="HW13" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
@@ -8558,8 +8698,23 @@
       <c r="HR14" s="13">
         <v>0</v>
       </c>
+      <c r="HS14" s="13">
+        <v>101500</v>
+      </c>
+      <c r="HT14" s="13">
+        <v>101520.420791</v>
+      </c>
+      <c r="HU14" s="13">
+        <v>101540.841577</v>
+      </c>
+      <c r="HV14" s="13">
+        <v>101602.103946</v>
+      </c>
+      <c r="HW14" s="13">
+        <v>101622.524737</v>
+      </c>
     </row>
-    <row r="15" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>25</v>
       </c>
@@ -9238,8 +9393,23 @@
       <c r="HR15" s="13">
         <v>0</v>
       </c>
+      <c r="HS15" s="13">
+        <v>0</v>
+      </c>
+      <c r="HT15" s="13">
+        <v>0</v>
+      </c>
+      <c r="HU15" s="13">
+        <v>0</v>
+      </c>
+      <c r="HV15" s="13">
+        <v>0</v>
+      </c>
+      <c r="HW15" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
@@ -9918,8 +10088,23 @@
       <c r="HR16" s="13">
         <v>0</v>
       </c>
+      <c r="HS16" s="13">
+        <v>0</v>
+      </c>
+      <c r="HT16" s="13">
+        <v>0</v>
+      </c>
+      <c r="HU16" s="13">
+        <v>0</v>
+      </c>
+      <c r="HV16" s="13">
+        <v>0</v>
+      </c>
+      <c r="HW16" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
@@ -10598,8 +10783,23 @@
       <c r="HR17" s="13">
         <v>0</v>
       </c>
+      <c r="HS17" s="13">
+        <v>0</v>
+      </c>
+      <c r="HT17" s="13">
+        <v>0</v>
+      </c>
+      <c r="HU17" s="13">
+        <v>0</v>
+      </c>
+      <c r="HV17" s="13">
+        <v>0</v>
+      </c>
+      <c r="HW17" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
@@ -11278,8 +11478,23 @@
       <c r="HR18" s="13">
         <v>0</v>
       </c>
+      <c r="HS18" s="13">
+        <v>0</v>
+      </c>
+      <c r="HT18" s="13">
+        <v>0</v>
+      </c>
+      <c r="HU18" s="13">
+        <v>0</v>
+      </c>
+      <c r="HV18" s="13">
+        <v>0</v>
+      </c>
+      <c r="HW18" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
@@ -11958,8 +12173,23 @@
       <c r="HR19" s="13">
         <v>0</v>
       </c>
+      <c r="HS19" s="13">
+        <v>0</v>
+      </c>
+      <c r="HT19" s="13">
+        <v>0</v>
+      </c>
+      <c r="HU19" s="13">
+        <v>0</v>
+      </c>
+      <c r="HV19" s="13">
+        <v>0</v>
+      </c>
+      <c r="HW19" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:226" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:231" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>11</v>
       </c>
@@ -12638,8 +12868,23 @@
       <c r="HR20" s="13">
         <v>0</v>
       </c>
+      <c r="HS20" s="13">
+        <v>0</v>
+      </c>
+      <c r="HT20" s="13">
+        <v>0</v>
+      </c>
+      <c r="HU20" s="13">
+        <v>0</v>
+      </c>
+      <c r="HV20" s="13">
+        <v>0</v>
+      </c>
+      <c r="HW20" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
@@ -13318,8 +13563,23 @@
       <c r="HR21" s="13">
         <v>0</v>
       </c>
+      <c r="HS21" s="13">
+        <v>0</v>
+      </c>
+      <c r="HT21" s="13">
+        <v>0</v>
+      </c>
+      <c r="HU21" s="13">
+        <v>0</v>
+      </c>
+      <c r="HV21" s="13">
+        <v>0</v>
+      </c>
+      <c r="HW21" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
@@ -13998,8 +14258,23 @@
       <c r="HR22" s="13">
         <v>434643.21051602543</v>
       </c>
+      <c r="HS22" s="13">
+        <v>435429.89261272817</v>
+      </c>
+      <c r="HT22" s="13">
+        <v>435371.74970357458</v>
+      </c>
+      <c r="HU22" s="13">
+        <v>435619.3425712419</v>
+      </c>
+      <c r="HV22" s="13">
+        <v>430608.12154032744</v>
+      </c>
+      <c r="HW22" s="13">
+        <v>428779.46535352373</v>
+      </c>
     </row>
-    <row r="23" spans="1:226" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:231" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="19" t="s">
         <v>4</v>
       </c>
@@ -14678,8 +14953,23 @@
       <c r="HR23" s="20">
         <v>1695064.9158371999</v>
       </c>
+      <c r="HS23" s="20">
+        <v>1790058.3086838</v>
+      </c>
+      <c r="HT23" s="20">
+        <v>1789265.5757076</v>
+      </c>
+      <c r="HU23" s="20">
+        <v>1786686.8547745002</v>
+      </c>
+      <c r="HV23" s="20">
+        <v>1795153.2256868996</v>
+      </c>
+      <c r="HW23" s="20">
+        <v>1799183.5754344</v>
+      </c>
     </row>
-    <row r="24" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>5</v>
       </c>
@@ -15358,8 +15648,23 @@
       <c r="HR24" s="13">
         <v>941735.88896190003</v>
       </c>
+      <c r="HS24" s="13">
+        <v>935521.83723629999</v>
+      </c>
+      <c r="HT24" s="13">
+        <v>932668.04417629994</v>
+      </c>
+      <c r="HU24" s="13">
+        <v>933019.12539479998</v>
+      </c>
+      <c r="HV24" s="13">
+        <v>928853.59757079999</v>
+      </c>
+      <c r="HW24" s="13">
+        <v>922964.67687079997</v>
+      </c>
     </row>
-    <row r="25" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>14</v>
       </c>
@@ -16038,8 +16343,23 @@
       <c r="HR25" s="13">
         <v>299492.17372660001</v>
       </c>
+      <c r="HS25" s="13">
+        <v>394223.21471049997</v>
+      </c>
+      <c r="HT25" s="13">
+        <v>398174.568058</v>
+      </c>
+      <c r="HU25" s="13">
+        <v>395871.45893680002</v>
+      </c>
+      <c r="HV25" s="13">
+        <v>400045.77124249999</v>
+      </c>
+      <c r="HW25" s="13">
+        <v>412733.57553970005</v>
+      </c>
     </row>
-    <row r="26" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
@@ -16718,8 +17038,23 @@
       <c r="HR26" s="13">
         <v>436211.41783970001</v>
       </c>
+      <c r="HS26" s="13">
+        <v>441596.99166270002</v>
+      </c>
+      <c r="HT26" s="13">
+        <v>442336.98781199998</v>
+      </c>
+      <c r="HU26" s="13">
+        <v>442115.41520820005</v>
+      </c>
+      <c r="HV26" s="13">
+        <v>452036.57373880001</v>
+      </c>
+      <c r="HW26" s="13">
+        <v>448952.56165359996</v>
+      </c>
     </row>
-    <row r="27" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>213</v>
       </c>
@@ -17062,8 +17397,23 @@
       <c r="HR27" s="13">
         <v>1.2020767999999999</v>
       </c>
+      <c r="HS27" s="13">
+        <v>1.2020767999999999</v>
+      </c>
+      <c r="HT27" s="13">
+        <v>1.2020767999999999</v>
+      </c>
+      <c r="HU27" s="13">
+        <v>1.1957666000000002</v>
+      </c>
+      <c r="HV27" s="13">
+        <v>1.1957666000000002</v>
+      </c>
+      <c r="HW27" s="13">
+        <v>1.1957666000000002</v>
+      </c>
     </row>
-    <row r="28" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>214</v>
       </c>
@@ -17406,8 +17756,23 @@
       <c r="HR28" s="13">
         <v>150.37514680000001</v>
       </c>
+      <c r="HS28" s="13">
+        <v>150.41019919999997</v>
+      </c>
+      <c r="HT28" s="13">
+        <v>228.28901930000001</v>
+      </c>
+      <c r="HU28" s="13">
+        <v>228.10964279999999</v>
+      </c>
+      <c r="HV28" s="13">
+        <v>228.55882550000001</v>
+      </c>
+      <c r="HW28" s="13">
+        <v>229.1027531</v>
+      </c>
     </row>
-    <row r="29" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>6</v>
       </c>
@@ -18086,8 +18451,23 @@
       <c r="HR29" s="13">
         <v>17473.858085399846</v>
       </c>
+      <c r="HS29" s="13">
+        <v>18564.652798300056</v>
+      </c>
+      <c r="HT29" s="13">
+        <v>15856.484565200064</v>
+      </c>
+      <c r="HU29" s="13">
+        <v>15451.549825300197</v>
+      </c>
+      <c r="HV29" s="13">
+        <v>13987.528542699625</v>
+      </c>
+      <c r="HW29" s="13">
+        <v>14302.462850600024</v>
+      </c>
     </row>
-    <row r="30" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>7</v>
       </c>
@@ -18766,8 +19146,23 @@
       <c r="HR30" s="13">
         <v>14328.4166774</v>
       </c>
+      <c r="HS30" s="13">
+        <v>16045.308724199998</v>
+      </c>
+      <c r="HT30" s="13">
+        <v>12544.973189900002</v>
+      </c>
+      <c r="HU30" s="13">
+        <v>11569.305451100001</v>
+      </c>
+      <c r="HV30" s="13">
+        <v>10115.568852800001</v>
+      </c>
+      <c r="HW30" s="13">
+        <v>10425.900176699999</v>
+      </c>
     </row>
-    <row r="31" spans="1:226" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:231" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -19446,8 +19841,23 @@
       <c r="HR31" s="13">
         <v>3145.4414079999997</v>
       </c>
+      <c r="HS31" s="13">
+        <v>2519.3440740999999</v>
+      </c>
+      <c r="HT31" s="13">
+        <v>3311.5113753000005</v>
+      </c>
+      <c r="HU31" s="13">
+        <v>3882.2443742</v>
+      </c>
+      <c r="HV31" s="13">
+        <v>3871.9596899000003</v>
+      </c>
+      <c r="HW31" s="13">
+        <v>3876.5626739000004</v>
+      </c>
     </row>
-    <row r="32" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="14"/>
       <c r="C32" s="14"/>
@@ -19674,8 +20084,13 @@
       <c r="HP32" s="14"/>
       <c r="HQ32" s="14"/>
       <c r="HR32" s="14"/>
+      <c r="HS32" s="14"/>
+      <c r="HT32" s="14"/>
+      <c r="HU32" s="14"/>
+      <c r="HV32" s="14"/>
+      <c r="HW32" s="14"/>
     </row>
-    <row r="33" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>15</v>
       </c>
@@ -19904,8 +20319,13 @@
       <c r="HP33" s="15"/>
       <c r="HQ33" s="15"/>
       <c r="HR33" s="15"/>
+      <c r="HS33" s="15"/>
+      <c r="HT33" s="15"/>
+      <c r="HU33" s="15"/>
+      <c r="HV33" s="15"/>
+      <c r="HW33" s="15"/>
     </row>
-    <row r="34" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" s="16"/>
       <c r="C34" s="16"/>
@@ -20132,8 +20552,13 @@
       <c r="HP34" s="16"/>
       <c r="HQ34" s="16"/>
       <c r="HR34" s="16"/>
+      <c r="HS34" s="16"/>
+      <c r="HT34" s="16"/>
+      <c r="HU34" s="16"/>
+      <c r="HV34" s="16"/>
+      <c r="HW34" s="16"/>
     </row>
-    <row r="35" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>26</v>
       </c>
@@ -21011,7 +21436,7 @@
         <v>-230.20401805522852</v>
       </c>
       <c r="HM35" s="14">
-        <f t="shared" ref="HM35:HR37" si="22">HM7-HL7</f>
+        <f t="shared" ref="HM35:HW37" si="22">HM7-HL7</f>
         <v>-5957.9455439161975</v>
       </c>
       <c r="HN35" s="14">
@@ -21034,8 +21459,28 @@
         <f t="shared" si="22"/>
         <v>2378.8110706228763</v>
       </c>
+      <c r="HS35" s="14">
+        <f t="shared" si="22"/>
+        <v>-8171.4610946025932</v>
+      </c>
+      <c r="HT35" s="14">
+        <f t="shared" si="22"/>
+        <v>2230.8482782533392</v>
+      </c>
+      <c r="HU35" s="14">
+        <f t="shared" si="22"/>
+        <v>6574.1674157330999</v>
+      </c>
+      <c r="HV35" s="14">
+        <f t="shared" si="22"/>
+        <v>11386.455398514052</v>
+      </c>
+      <c r="HW35" s="14">
+        <f t="shared" si="22"/>
+        <v>36089.849999903701</v>
+      </c>
     </row>
-    <row r="36" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>21</v>
       </c>
@@ -21936,8 +22381,28 @@
         <f t="shared" si="22"/>
         <v>-34191.724067022791</v>
       </c>
+      <c r="HS36" s="14">
+        <f t="shared" si="22"/>
+        <v>103164.85394120275</v>
+      </c>
+      <c r="HT36" s="14">
+        <f t="shared" si="22"/>
+        <v>-3023.5812544533983</v>
+      </c>
+      <c r="HU36" s="14">
+        <f t="shared" si="22"/>
+        <v>-9152.8883488328429</v>
+      </c>
+      <c r="HV36" s="14">
+        <f t="shared" si="22"/>
+        <v>-2920.0844861146761</v>
+      </c>
+      <c r="HW36" s="14">
+        <f t="shared" si="22"/>
+        <v>-32059.500252403319</v>
+      </c>
     </row>
-    <row r="37" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>2</v>
       </c>
@@ -22838,8 +23303,28 @@
         <f t="shared" si="22"/>
         <v>-36630.306644000055</v>
       </c>
+      <c r="HS37" s="14">
+        <f t="shared" si="22"/>
+        <v>-18750.033145099937</v>
+      </c>
+      <c r="HT37" s="14">
+        <f t="shared" si="22"/>
+        <v>-2973.629749200074</v>
+      </c>
+      <c r="HU37" s="14">
+        <f t="shared" si="22"/>
+        <v>-9710.9414056999958</v>
+      </c>
+      <c r="HV37" s="14">
+        <f t="shared" si="22"/>
+        <v>1663.209764499974</v>
+      </c>
+      <c r="HW37" s="14">
+        <f t="shared" si="22"/>
+        <v>-36839.982874399924</v>
+      </c>
     </row>
-    <row r="38" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>3</v>
       </c>
@@ -23713,7 +24198,7 @@
         <v>98.33037209988106</v>
       </c>
       <c r="HL38" s="14">
-        <f t="shared" ref="HL38:HR43" si="51">HL10-HK10</f>
+        <f t="shared" ref="HL38:HW43" si="51">HL10-HK10</f>
         <v>-20382.481825899915</v>
       </c>
       <c r="HM38" s="14">
@@ -23740,8 +24225,28 @@
         <f t="shared" si="51"/>
         <v>117.87639699992724</v>
       </c>
+      <c r="HS38" s="14">
+        <f t="shared" si="51"/>
+        <v>121128.2049896</v>
+      </c>
+      <c r="HT38" s="14">
+        <f t="shared" si="51"/>
+        <v>8.1914039002731442</v>
+      </c>
+      <c r="HU38" s="14">
+        <f t="shared" si="51"/>
+        <v>310.46018919977359</v>
+      </c>
+      <c r="HV38" s="14">
+        <f t="shared" si="51"/>
+        <v>427.92678029998206</v>
+      </c>
+      <c r="HW38" s="14">
+        <f t="shared" si="51"/>
+        <v>6609.1388088001404</v>
+      </c>
     </row>
-    <row r="39" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>17</v>
       </c>
@@ -24642,8 +25147,28 @@
         <f t="shared" si="51"/>
         <v>69.954278000048362</v>
       </c>
+      <c r="HS39" s="14">
+        <f t="shared" si="51"/>
+        <v>121080.27434299997</v>
+      </c>
+      <c r="HT39" s="14">
+        <f t="shared" si="51"/>
+        <v>94.677922000002582</v>
+      </c>
+      <c r="HU39" s="14">
+        <f t="shared" si="51"/>
+        <v>94.677919999987353</v>
+      </c>
+      <c r="HV39" s="14">
+        <f t="shared" si="51"/>
+        <v>284.03375900001265</v>
+      </c>
+      <c r="HW39" s="14">
+        <f t="shared" si="51"/>
+        <v>94.677925000025425</v>
+      </c>
     </row>
-    <row r="40" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>22</v>
       </c>
@@ -25544,8 +26069,28 @@
         <f t="shared" si="51"/>
         <v>69.954277999990154</v>
       </c>
+      <c r="HS40" s="14">
+        <f t="shared" si="51"/>
+        <v>19580.274343000026</v>
+      </c>
+      <c r="HT40" s="14">
+        <f t="shared" si="51"/>
+        <v>74.257130999991205</v>
+      </c>
+      <c r="HU40" s="14">
+        <f t="shared" si="51"/>
+        <v>74.257134000014048</v>
+      </c>
+      <c r="HV40" s="14">
+        <f t="shared" si="51"/>
+        <v>222.77139000000898</v>
+      </c>
+      <c r="HW40" s="14">
+        <f t="shared" si="51"/>
+        <v>74.257134000014048</v>
+      </c>
     </row>
-    <row r="41" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>23</v>
       </c>
@@ -26446,8 +26991,28 @@
         <f t="shared" si="51"/>
         <v>0</v>
       </c>
+      <c r="HS41" s="14">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="HT41" s="14">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="HU41" s="14">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="HV41" s="14">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="HW41" s="14">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="42" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>24</v>
       </c>
@@ -27348,8 +27913,28 @@
         <f t="shared" si="51"/>
         <v>0</v>
       </c>
+      <c r="HS42" s="14">
+        <f t="shared" si="51"/>
+        <v>101500</v>
+      </c>
+      <c r="HT42" s="14">
+        <f t="shared" si="51"/>
+        <v>20.420790999996825</v>
+      </c>
+      <c r="HU42" s="14">
+        <f t="shared" si="51"/>
+        <v>20.420786000002408</v>
+      </c>
+      <c r="HV42" s="14">
+        <f t="shared" si="51"/>
+        <v>61.262369000003673</v>
+      </c>
+      <c r="HW42" s="14">
+        <f t="shared" si="51"/>
+        <v>20.420790999996825</v>
+      </c>
     </row>
-    <row r="43" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>25</v>
       </c>
@@ -28250,8 +28835,28 @@
         <f t="shared" si="51"/>
         <v>0</v>
       </c>
+      <c r="HS43" s="14">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="HT43" s="14">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="HU43" s="14">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="HV43" s="14">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="HW43" s="14">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="44" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>9</v>
       </c>
@@ -28977,7 +29582,7 @@
         <v>0</v>
       </c>
       <c r="GA44" s="14">
-        <f t="shared" ref="GA44:HR44" si="106">GA16-FZ16</f>
+        <f t="shared" ref="GA44:HW44" si="106">GA16-FZ16</f>
         <v>0</v>
       </c>
       <c r="GB44" s="14">
@@ -29152,8 +29757,28 @@
         <f t="shared" si="106"/>
         <v>0</v>
       </c>
+      <c r="HS44" s="14">
+        <f t="shared" si="106"/>
+        <v>0</v>
+      </c>
+      <c r="HT44" s="14">
+        <f t="shared" si="106"/>
+        <v>0</v>
+      </c>
+      <c r="HU44" s="14">
+        <f t="shared" si="106"/>
+        <v>0</v>
+      </c>
+      <c r="HV44" s="14">
+        <f t="shared" si="106"/>
+        <v>0</v>
+      </c>
+      <c r="HW44" s="14">
+        <f t="shared" si="106"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="45" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>10</v>
       </c>
@@ -29911,7 +30536,7 @@
         <v>1000.1639344</v>
       </c>
       <c r="GI45" s="14">
-        <f t="shared" ref="GI45:HR49" si="116">-(GI17-GH17)</f>
+        <f t="shared" ref="GI45:HW49" si="116">-(GI17-GH17)</f>
         <v>-1000.1639344</v>
       </c>
       <c r="GJ45" s="14">
@@ -30054,8 +30679,28 @@
         <f t="shared" si="116"/>
         <v>0</v>
       </c>
+      <c r="HS45" s="14">
+        <f t="shared" si="116"/>
+        <v>0</v>
+      </c>
+      <c r="HT45" s="14">
+        <f t="shared" si="116"/>
+        <v>0</v>
+      </c>
+      <c r="HU45" s="14">
+        <f t="shared" si="116"/>
+        <v>0</v>
+      </c>
+      <c r="HV45" s="14">
+        <f t="shared" si="116"/>
+        <v>0</v>
+      </c>
+      <c r="HW45" s="14">
+        <f t="shared" si="116"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="46" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>12</v>
       </c>
@@ -30956,8 +31601,28 @@
         <f t="shared" si="116"/>
         <v>0</v>
       </c>
+      <c r="HS46" s="14">
+        <f t="shared" si="116"/>
+        <v>0</v>
+      </c>
+      <c r="HT46" s="14">
+        <f t="shared" si="116"/>
+        <v>0</v>
+      </c>
+      <c r="HU46" s="14">
+        <f t="shared" si="116"/>
+        <v>0</v>
+      </c>
+      <c r="HV46" s="14">
+        <f t="shared" si="116"/>
+        <v>0</v>
+      </c>
+      <c r="HW46" s="14">
+        <f t="shared" si="116"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="47" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>18</v>
       </c>
@@ -31858,8 +32523,28 @@
         <f t="shared" si="116"/>
         <v>0</v>
       </c>
+      <c r="HS47" s="14">
+        <f t="shared" si="116"/>
+        <v>0</v>
+      </c>
+      <c r="HT47" s="14">
+        <f t="shared" si="116"/>
+        <v>0</v>
+      </c>
+      <c r="HU47" s="14">
+        <f t="shared" si="116"/>
+        <v>0</v>
+      </c>
+      <c r="HV47" s="14">
+        <f t="shared" si="116"/>
+        <v>0</v>
+      </c>
+      <c r="HW47" s="14">
+        <f t="shared" si="116"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>11</v>
       </c>
@@ -32760,8 +33445,28 @@
         <f t="shared" si="116"/>
         <v>0</v>
       </c>
+      <c r="HS48" s="14">
+        <f t="shared" si="116"/>
+        <v>0</v>
+      </c>
+      <c r="HT48" s="14">
+        <f t="shared" si="116"/>
+        <v>0</v>
+      </c>
+      <c r="HU48" s="14">
+        <f t="shared" si="116"/>
+        <v>0</v>
+      </c>
+      <c r="HV48" s="14">
+        <f t="shared" si="116"/>
+        <v>0</v>
+      </c>
+      <c r="HW48" s="14">
+        <f t="shared" si="116"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="49" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>16</v>
       </c>
@@ -33662,8 +34367,28 @@
         <f t="shared" si="116"/>
         <v>0</v>
       </c>
+      <c r="HS49" s="14">
+        <f t="shared" si="116"/>
+        <v>0</v>
+      </c>
+      <c r="HT49" s="14">
+        <f t="shared" si="116"/>
+        <v>0</v>
+      </c>
+      <c r="HU49" s="14">
+        <f t="shared" si="116"/>
+        <v>0</v>
+      </c>
+      <c r="HV49" s="14">
+        <f t="shared" si="116"/>
+        <v>0</v>
+      </c>
+      <c r="HW49" s="14">
+        <f t="shared" si="116"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="50" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>20</v>
       </c>
@@ -34421,7 +35146,7 @@
         <v>-7970.1339649318252</v>
       </c>
       <c r="GI50" s="14">
-        <f t="shared" ref="GI50:HR54" si="163">GI22-GH22</f>
+        <f t="shared" ref="GI50:HW54" si="163">GI22-GH22</f>
         <v>1639.8867724001175</v>
       </c>
       <c r="GJ50" s="14">
@@ -34564,8 +35289,28 @@
         <f t="shared" si="163"/>
         <v>2320.7061799773946</v>
       </c>
+      <c r="HS50" s="14">
+        <f t="shared" si="163"/>
+        <v>786.68209670274518</v>
+      </c>
+      <c r="HT50" s="14">
+        <f t="shared" si="163"/>
+        <v>-58.142909153597429</v>
+      </c>
+      <c r="HU50" s="14">
+        <f t="shared" si="163"/>
+        <v>247.59286766732112</v>
+      </c>
+      <c r="HV50" s="14">
+        <f t="shared" si="163"/>
+        <v>-5011.2210309144575</v>
+      </c>
+      <c r="HW50" s="14">
+        <f t="shared" si="163"/>
+        <v>-1828.6561868037097</v>
+      </c>
     </row>
-    <row r="51" spans="1:226" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:231" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="19" t="s">
         <v>4</v>
       </c>
@@ -35466,8 +36211,28 @@
         <f t="shared" si="163"/>
         <v>-31812.912996399915</v>
       </c>
+      <c r="HS51" s="22">
+        <f t="shared" si="163"/>
+        <v>94993.392846600153</v>
+      </c>
+      <c r="HT51" s="22">
+        <f t="shared" si="163"/>
+        <v>-792.73297620005906</v>
+      </c>
+      <c r="HU51" s="22">
+        <f t="shared" si="163"/>
+        <v>-2578.720933099743</v>
+      </c>
+      <c r="HV51" s="22">
+        <f t="shared" si="163"/>
+        <v>8466.3709123993758</v>
+      </c>
+      <c r="HW51" s="22">
+        <f t="shared" si="163"/>
+        <v>4030.3497475003824</v>
+      </c>
     </row>
-    <row r="52" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>5</v>
       </c>
@@ -36368,8 +37133,28 @@
         <f t="shared" si="163"/>
         <v>-3421.5051499999827</v>
       </c>
+      <c r="HS52" s="14">
+        <f t="shared" si="163"/>
+        <v>-6214.0517256000312</v>
+      </c>
+      <c r="HT52" s="14">
+        <f t="shared" si="163"/>
+        <v>-2853.7930600000545</v>
+      </c>
+      <c r="HU52" s="14">
+        <f t="shared" si="163"/>
+        <v>351.08121850003954</v>
+      </c>
+      <c r="HV52" s="14">
+        <f t="shared" si="163"/>
+        <v>-4165.5278239999898</v>
+      </c>
+      <c r="HW52" s="14">
+        <f t="shared" si="163"/>
+        <v>-5888.920700000017</v>
+      </c>
     </row>
-    <row r="53" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>14</v>
       </c>
@@ -37270,8 +38055,28 @@
         <f t="shared" si="163"/>
         <v>-34369.818471499952</v>
       </c>
+      <c r="HS53" s="14">
+        <f t="shared" si="163"/>
+        <v>94731.040983899962</v>
+      </c>
+      <c r="HT53" s="14">
+        <f t="shared" si="163"/>
+        <v>3951.3533475000295</v>
+      </c>
+      <c r="HU53" s="14">
+        <f t="shared" si="163"/>
+        <v>-2303.1091211999883</v>
+      </c>
+      <c r="HV53" s="14">
+        <f t="shared" si="163"/>
+        <v>4174.3123056999757</v>
+      </c>
+      <c r="HW53" s="14">
+        <f t="shared" si="163"/>
+        <v>12687.804297200055</v>
+      </c>
     </row>
-    <row r="54" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>13</v>
       </c>
@@ -38172,8 +38977,28 @@
         <f t="shared" si="163"/>
         <v>3612.9173938999884</v>
       </c>
+      <c r="HS54" s="14">
+        <f t="shared" si="163"/>
+        <v>5385.5738230000134</v>
+      </c>
+      <c r="HT54" s="14">
+        <f t="shared" si="163"/>
+        <v>739.99614929995732</v>
+      </c>
+      <c r="HU54" s="14">
+        <f t="shared" si="163"/>
+        <v>-221.57260379992658</v>
+      </c>
+      <c r="HV54" s="14">
+        <f t="shared" si="163"/>
+        <v>9921.1585305999615</v>
+      </c>
+      <c r="HW54" s="14">
+        <f t="shared" si="163"/>
+        <v>-3084.0120852000546</v>
+      </c>
     </row>
-    <row r="55" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>209</v>
       </c>
@@ -38349,7 +39174,7 @@
         <v>0</v>
       </c>
       <c r="FN55" s="14">
-        <f t="shared" ref="FN55:HR55" si="202">FN27-FM27</f>
+        <f t="shared" ref="FN55:HW55" si="202">FN27-FM27</f>
         <v>1.1020768000000001</v>
       </c>
       <c r="FO55" s="14">
@@ -38576,8 +39401,28 @@
         <f t="shared" si="202"/>
         <v>0</v>
       </c>
+      <c r="HS55" s="14">
+        <f t="shared" si="202"/>
+        <v>0</v>
+      </c>
+      <c r="HT55" s="14">
+        <f t="shared" si="202"/>
+        <v>0</v>
+      </c>
+      <c r="HU55" s="14">
+        <f t="shared" si="202"/>
+        <v>-6.3101999999997105E-3</v>
+      </c>
+      <c r="HV55" s="14">
+        <f t="shared" si="202"/>
+        <v>0</v>
+      </c>
+      <c r="HW55" s="14">
+        <f t="shared" si="202"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="56" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>210</v>
       </c>
@@ -38753,7 +39598,7 @@
         <v>0</v>
       </c>
       <c r="FN56" s="14">
-        <f t="shared" ref="FN56:HR56" si="203">FN28-FM28</f>
+        <f t="shared" ref="FN56:HW56" si="203">FN28-FM28</f>
         <v>143.637857</v>
       </c>
       <c r="FO56" s="14">
@@ -38980,8 +39825,28 @@
         <f t="shared" si="203"/>
         <v>8.8615400000009004E-2</v>
       </c>
+      <c r="HS56" s="14">
+        <f t="shared" si="203"/>
+        <v>3.5052399999955242E-2</v>
+      </c>
+      <c r="HT56" s="14">
+        <f t="shared" si="203"/>
+        <v>77.878820100000041</v>
+      </c>
+      <c r="HU56" s="14">
+        <f t="shared" si="203"/>
+        <v>-0.17937650000001781</v>
+      </c>
+      <c r="HV56" s="14">
+        <f t="shared" si="203"/>
+        <v>0.44918270000002281</v>
+      </c>
+      <c r="HW56" s="14">
+        <f t="shared" si="203"/>
+        <v>0.5439275999999893</v>
+      </c>
     </row>
-    <row r="57" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>6</v>
       </c>
@@ -39655,7 +40520,7 @@
         <v>1333.7321843000245</v>
       </c>
       <c r="FN57" s="14">
-        <f t="shared" ref="FN57:HR57" si="218">FN29-FM29</f>
+        <f t="shared" ref="FN57:HW57" si="218">FN29-FM29</f>
         <v>40.069721600106277</v>
       </c>
       <c r="FO57" s="14">
@@ -39882,8 +40747,28 @@
         <f t="shared" si="218"/>
         <v>2365.4046158000292</v>
       </c>
+      <c r="HS57" s="14">
+        <f t="shared" si="218"/>
+        <v>1090.7947129002096</v>
+      </c>
+      <c r="HT57" s="14">
+        <f t="shared" si="218"/>
+        <v>-2708.168233099992</v>
+      </c>
+      <c r="HU57" s="14">
+        <f t="shared" si="218"/>
+        <v>-404.93473989986705</v>
+      </c>
+      <c r="HV57" s="14">
+        <f t="shared" si="218"/>
+        <v>-1464.0212826005718</v>
+      </c>
+      <c r="HW57" s="14">
+        <f t="shared" si="218"/>
+        <v>314.93430790039929</v>
+      </c>
     </row>
-    <row r="58" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>7</v>
       </c>
@@ -40557,7 +41442,7 @@
         <v>85.767450500003179</v>
       </c>
       <c r="FN58" s="14">
-        <f t="shared" ref="FN58:HR58" si="220">FN30-FM30</f>
+        <f t="shared" ref="FN58:HW58" si="220">FN30-FM30</f>
         <v>36.631565799998498</v>
       </c>
       <c r="FO58" s="14">
@@ -40784,8 +41669,28 @@
         <f t="shared" si="220"/>
         <v>3614.6010722999981</v>
       </c>
+      <c r="HS58" s="14">
+        <f t="shared" si="220"/>
+        <v>1716.8920467999978</v>
+      </c>
+      <c r="HT58" s="14">
+        <f t="shared" si="220"/>
+        <v>-3500.3355342999967</v>
+      </c>
+      <c r="HU58" s="14">
+        <f t="shared" si="220"/>
+        <v>-975.66773880000073</v>
+      </c>
+      <c r="HV58" s="14">
+        <f t="shared" si="220"/>
+        <v>-1453.7365983</v>
+      </c>
+      <c r="HW58" s="14">
+        <f t="shared" si="220"/>
+        <v>310.3313238999981</v>
+      </c>
     </row>
-    <row r="59" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>8</v>
       </c>
@@ -41459,7 +42364,7 @@
         <v>1247.9647337999995</v>
       </c>
       <c r="FN59" s="14">
-        <f t="shared" ref="FN59:HR59" si="222">FN31-FM31</f>
+        <f t="shared" ref="FN59:HW59" si="222">FN31-FM31</f>
         <v>3.4381558000004588</v>
       </c>
       <c r="FO59" s="14">
@@ -41686,19 +42591,39 @@
         <f t="shared" si="222"/>
         <v>-1249.1964565000007</v>
       </c>
+      <c r="HS59" s="14">
+        <f t="shared" si="222"/>
+        <v>-626.09733389999974</v>
+      </c>
+      <c r="HT59" s="14">
+        <f t="shared" si="222"/>
+        <v>792.16730120000057</v>
+      </c>
+      <c r="HU59" s="14">
+        <f t="shared" si="222"/>
+        <v>570.73299889999953</v>
+      </c>
+      <c r="HV59" s="14">
+        <f t="shared" si="222"/>
+        <v>-10.284684299999753</v>
+      </c>
+      <c r="HW59" s="14">
+        <f t="shared" si="222"/>
+        <v>4.6029840000001059</v>
+      </c>
     </row>
-    <row r="60" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
     </row>
-    <row r="61" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A61" s="17"/>
     </row>
-    <row r="62" spans="1:226" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:231" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="25" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="63" spans="1:226" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A63" s="26" t="s">
         <v>216</v>
       </c>
@@ -41842,13 +42767,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63D1FEF7-8411-4E12-8BC2-90C8F09824F5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A657985-5356-4E74-B068-A6C75E213039}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0847128-EC15-4309-8357-F70482C70CF4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1AF02399-D6B9-40C8-9AAE-00911610B26D}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9B630E1-BB59-47FC-A9BB-9F0EB94A21D0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6608200-0E4B-4A04-811C-D2771162E960}"/>
 </file>
</xml_diff>